<commit_message>
preenchimento dos preços dos alimentos
</commit_message>
<xml_diff>
--- a/alimentosCompleto.xlsx
+++ b/alimentosCompleto.xlsx
@@ -265,7 +265,7 @@
     <t xml:space="preserve">pera</t>
   </si>
   <si>
-    <t xml:space="preserve">pessogo</t>
+    <t xml:space="preserve">pessego</t>
   </si>
   <si>
     <t xml:space="preserve">tangerina</t>
@@ -388,11 +388,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -522,7 +522,7 @@
   <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -530,7 +530,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -614,9 +614,15 @@
       <c r="K2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="L2" s="3" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O2" s="2" t="n">
         <v>4</v>
       </c>
@@ -655,9 +661,15 @@
       <c r="K3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="L3" s="3" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O3" s="2" t="n">
         <v>4</v>
       </c>
@@ -696,9 +708,15 @@
       <c r="K4" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="L4" s="3" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O4" s="2" t="n">
         <v>4</v>
       </c>
@@ -737,9 +755,15 @@
       <c r="K5" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="L5" s="3" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O5" s="2" t="n">
         <v>4</v>
       </c>
@@ -778,9 +802,15 @@
       <c r="K6" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="L6" s="3" t="n">
+        <v>0.958</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O6" s="2" t="n">
         <v>4</v>
       </c>
@@ -819,9 +849,15 @@
       <c r="K7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+      <c r="L7" s="3" t="n">
+        <v>0.289</v>
+      </c>
+      <c r="M7" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N7" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O7" s="2" t="n">
         <v>4</v>
       </c>
@@ -860,9 +896,15 @@
       <c r="K8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="L8" s="3" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="M8" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N8" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O8" s="2" t="n">
         <v>4</v>
       </c>
@@ -901,9 +943,15 @@
       <c r="K9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="L9" s="3" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="M9" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N9" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O9" s="2" t="n">
         <v>4</v>
       </c>
@@ -942,9 +990,15 @@
       <c r="K10" s="2" t="n">
         <v>272</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+      <c r="L10" s="3" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="M10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N10" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O10" s="2" t="n">
         <v>4</v>
       </c>
@@ -983,9 +1037,15 @@
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="L11" s="3" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O11" s="2" t="n">
         <v>4</v>
       </c>
@@ -1024,9 +1084,15 @@
       <c r="K12" s="2" t="n">
         <v>594</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="L12" s="3" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O12" s="2" t="n">
         <v>4</v>
       </c>
@@ -1065,9 +1131,15 @@
       <c r="K13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="L13" s="3" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="M13" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O13" s="2" t="n">
         <v>4</v>
       </c>
@@ -1106,9 +1178,15 @@
       <c r="K14" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="L14" s="3" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="M14" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N14" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O14" s="2" t="n">
         <v>4</v>
       </c>
@@ -1147,9 +1225,15 @@
       <c r="K15" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="L15" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M15" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N15" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O15" s="2" t="n">
         <v>4</v>
       </c>
@@ -1188,9 +1272,15 @@
       <c r="K16" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="L16" s="3" t="n">
+        <v>0.699</v>
+      </c>
+      <c r="M16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N16" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O16" s="2" t="n">
         <v>4</v>
       </c>
@@ -1229,9 +1319,15 @@
       <c r="K17" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="L17" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N17" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O17" s="2" t="n">
         <v>3</v>
       </c>
@@ -1270,9 +1366,15 @@
       <c r="K18" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="L18" s="3" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="M18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O18" s="2" t="n">
         <v>3</v>
       </c>
@@ -1311,9 +1413,15 @@
       <c r="K19" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="L19" s="3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="M19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N19" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O19" s="2" t="n">
         <v>3</v>
       </c>
@@ -1352,9 +1460,15 @@
       <c r="K20" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="L20" s="3" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="M20" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N20" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O20" s="2" t="n">
         <v>3</v>
       </c>
@@ -1393,9 +1507,15 @@
       <c r="K21" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
+      <c r="L21" s="3" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="M21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N21" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O21" s="2" t="n">
         <v>3</v>
       </c>
@@ -1434,9 +1554,15 @@
       <c r="K22" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
+      <c r="L22" s="3" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="M22" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N22" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O22" s="2" t="n">
         <v>3</v>
       </c>
@@ -1475,9 +1601,15 @@
       <c r="K23" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="L23" s="3" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="M23" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N23" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O23" s="2" t="n">
         <v>3</v>
       </c>
@@ -1516,9 +1648,15 @@
       <c r="K24" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="L24" s="3" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="M24" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N24" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O24" s="2" t="n">
         <v>3</v>
       </c>
@@ -1557,9 +1695,15 @@
       <c r="K25" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="L25" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M25" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N25" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O25" s="2" t="n">
         <v>3</v>
       </c>
@@ -1598,9 +1742,15 @@
       <c r="K26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
+      <c r="L26" s="3" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="M26" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N26" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O26" s="2" t="n">
         <v>3</v>
       </c>
@@ -1639,9 +1789,15 @@
       <c r="K27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="L27" s="3" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="M27" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N27" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O27" s="2" t="n">
         <v>3</v>
       </c>
@@ -1680,9 +1836,15 @@
       <c r="K28" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="L28" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M28" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N28" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O28" s="2" t="n">
         <v>3</v>
       </c>
@@ -1721,9 +1883,15 @@
       <c r="K29" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
+      <c r="L29" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M29" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N29" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O29" s="2" t="n">
         <v>3</v>
       </c>
@@ -1762,9 +1930,15 @@
       <c r="K30" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
+      <c r="L30" s="3" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="M30" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N30" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O30" s="2" t="n">
         <v>3</v>
       </c>
@@ -1803,9 +1977,15 @@
       <c r="K31" s="2" t="n">
         <v>563</v>
       </c>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
+      <c r="L31" s="3" t="n">
+        <v>4.058</v>
+      </c>
+      <c r="M31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N31" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O31" s="2" t="n">
         <v>3</v>
       </c>
@@ -1844,9 +2024,15 @@
       <c r="K32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
+      <c r="L32" s="3" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N32" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O32" s="2" t="n">
         <v>3</v>
       </c>
@@ -1885,9 +2071,15 @@
       <c r="K33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
+      <c r="L33" s="3" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="M33" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N33" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O33" s="2" t="n">
         <v>3</v>
       </c>
@@ -1926,9 +2118,15 @@
       <c r="K34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
+      <c r="L34" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N34" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O34" s="2" t="n">
         <v>3</v>
       </c>
@@ -1967,9 +2165,15 @@
       <c r="K35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="L35" s="3" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="M35" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N35" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O35" s="2" t="n">
         <v>3</v>
       </c>
@@ -2008,9 +2212,15 @@
       <c r="K36" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
+      <c r="L36" s="3" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="M36" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N36" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O36" s="2" t="n">
         <v>3</v>
       </c>
@@ -2049,9 +2259,15 @@
       <c r="K37" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
+      <c r="L37" s="3" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="M37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N37" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O37" s="2" t="n">
         <v>3</v>
       </c>
@@ -2090,9 +2306,15 @@
       <c r="K38" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
+      <c r="L38" s="3" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="M38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N38" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O38" s="2" t="n">
         <v>3</v>
       </c>
@@ -2131,9 +2353,15 @@
       <c r="K39" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
+      <c r="L39" s="3" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="M39" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N39" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O39" s="2" t="n">
         <v>3</v>
       </c>
@@ -2172,9 +2400,15 @@
       <c r="K40" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
+      <c r="L40" s="3" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="M40" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N40" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O40" s="2" t="n">
         <v>3</v>
       </c>
@@ -2213,9 +2447,15 @@
       <c r="K41" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
+      <c r="L41" s="3" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="M41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N41" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O41" s="2" t="n">
         <v>3</v>
       </c>
@@ -2254,9 +2494,15 @@
       <c r="K42" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
+      <c r="L42" s="3" t="n">
+        <v>8.63</v>
+      </c>
+      <c r="M42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N42" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O42" s="2" t="n">
         <v>3</v>
       </c>
@@ -2295,9 +2541,15 @@
       <c r="K43" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
+      <c r="L43" s="3" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="M43" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N43" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O43" s="2" t="n">
         <v>3</v>
       </c>
@@ -2336,9 +2588,15 @@
       <c r="K44" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
+      <c r="L44" s="3" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="M44" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N44" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O44" s="2" t="n">
         <v>3</v>
       </c>
@@ -2377,9 +2635,15 @@
       <c r="K45" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
+      <c r="L45" s="3" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="M45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N45" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O45" s="2" t="n">
         <v>3</v>
       </c>
@@ -2418,9 +2682,15 @@
       <c r="K46" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
+      <c r="L46" s="3" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="M46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N46" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O46" s="2" t="n">
         <v>2</v>
       </c>
@@ -2459,9 +2729,15 @@
       <c r="K47" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
+      <c r="L47" s="3" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="M47" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N47" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O47" s="2" t="n">
         <v>2</v>
       </c>
@@ -2500,9 +2776,15 @@
       <c r="K48" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
+      <c r="L48" s="3" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="M48" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N48" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O48" s="2" t="n">
         <v>2</v>
       </c>
@@ -2541,9 +2823,15 @@
       <c r="K49" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
+      <c r="L49" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M49" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N49" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O49" s="2" t="n">
         <v>2</v>
       </c>
@@ -2582,9 +2870,15 @@
       <c r="K50" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
+      <c r="L50" s="3" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="M50" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N50" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O50" s="2" t="n">
         <v>2</v>
       </c>
@@ -2623,9 +2917,15 @@
       <c r="K51" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
+      <c r="L51" s="3" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="M51" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N51" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O51" s="2" t="n">
         <v>2</v>
       </c>
@@ -2664,9 +2964,15 @@
       <c r="K52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
+      <c r="L52" s="3" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="M52" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N52" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O52" s="2" t="n">
         <v>2</v>
       </c>
@@ -2705,9 +3011,15 @@
       <c r="K53" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
+      <c r="L53" s="3" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="M53" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N53" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O53" s="2" t="n">
         <v>2</v>
       </c>
@@ -2746,9 +3058,15 @@
       <c r="K54" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
+      <c r="L54" s="3" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N54" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O54" s="2" t="n">
         <v>2</v>
       </c>
@@ -2787,9 +3105,15 @@
       <c r="K55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
+      <c r="L55" s="3" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="M55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N55" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O55" s="2" t="n">
         <v>2</v>
       </c>
@@ -2828,9 +3152,15 @@
       <c r="K56" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
+      <c r="L56" s="3" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="M56" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N56" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O56" s="2" t="n">
         <v>2</v>
       </c>
@@ -2869,9 +3199,15 @@
       <c r="K57" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
+      <c r="L57" s="3" t="n">
+        <v>0.298</v>
+      </c>
+      <c r="M57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N57" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O57" s="2" t="n">
         <v>2</v>
       </c>
@@ -2910,9 +3246,15 @@
       <c r="K58" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
+      <c r="L58" s="3" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="M58" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N58" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O58" s="2" t="n">
         <v>2</v>
       </c>
@@ -2951,9 +3293,15 @@
       <c r="K59" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
+      <c r="L59" s="3" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="M59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N59" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O59" s="2" t="n">
         <v>2</v>
       </c>
@@ -2992,9 +3340,15 @@
       <c r="K60" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
+      <c r="L60" s="3" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="M60" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N60" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O60" s="2" t="n">
         <v>2</v>
       </c>
@@ -3033,9 +3387,15 @@
       <c r="K61" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="3"/>
+      <c r="L61" s="3" t="n">
+        <v>2.268</v>
+      </c>
+      <c r="M61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N61" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O61" s="2" t="n">
         <v>2</v>
       </c>
@@ -3074,9 +3434,15 @@
       <c r="K62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="3"/>
+      <c r="L62" s="3" t="n">
+        <v>0.299</v>
+      </c>
+      <c r="M62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N62" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O62" s="2" t="n">
         <v>2</v>
       </c>
@@ -3115,9 +3481,15 @@
       <c r="K63" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
-      <c r="N63" s="3"/>
+      <c r="L63" s="3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M63" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N63" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O63" s="2" t="n">
         <v>2</v>
       </c>
@@ -3156,9 +3528,15 @@
       <c r="K64" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
+      <c r="L64" s="3" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="M64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N64" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O64" s="2" t="n">
         <v>2</v>
       </c>
@@ -3197,9 +3575,15 @@
       <c r="K65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
+      <c r="L65" s="3" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="M65" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N65" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O65" s="2" t="n">
         <v>2</v>
       </c>
@@ -3238,9 +3622,15 @@
       <c r="K66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
+      <c r="L66" s="3" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="M66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N66" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O66" s="2" t="n">
         <v>2</v>
       </c>
@@ -3279,9 +3669,15 @@
       <c r="K67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="3"/>
+      <c r="L67" s="3" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="M67" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N67" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O67" s="2" t="n">
         <v>2</v>
       </c>
@@ -3320,9 +3716,15 @@
       <c r="K68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
-      <c r="N68" s="3"/>
+      <c r="L68" s="3" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="M68" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N68" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O68" s="2" t="n">
         <v>2</v>
       </c>
@@ -3361,9 +3763,15 @@
       <c r="K69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L69" s="3"/>
-      <c r="M69" s="3"/>
-      <c r="N69" s="3"/>
+      <c r="L69" s="3" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="M69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N69" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O69" s="2" t="n">
         <v>2</v>
       </c>
@@ -3402,9 +3810,15 @@
       <c r="K70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
-      <c r="N70" s="3"/>
+      <c r="L70" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M70" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N70" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O70" s="2" t="n">
         <v>2</v>
       </c>
@@ -3443,9 +3857,15 @@
       <c r="K71" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="L71" s="3"/>
-      <c r="M71" s="3"/>
-      <c r="N71" s="3"/>
+      <c r="L71" s="3" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="M71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N71" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O71" s="2" t="n">
         <v>1</v>
       </c>
@@ -3484,9 +3904,15 @@
       <c r="K72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L72" s="3"/>
-      <c r="M72" s="3"/>
-      <c r="N72" s="3"/>
+      <c r="L72" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N72" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O72" s="2" t="n">
         <v>1</v>
       </c>
@@ -3525,9 +3951,15 @@
       <c r="K73" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="L73" s="3"/>
-      <c r="M73" s="3"/>
-      <c r="N73" s="3"/>
+      <c r="L73" s="3" t="n">
+        <v>2.179</v>
+      </c>
+      <c r="M73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N73" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O73" s="2" t="n">
         <v>1</v>
       </c>
@@ -3566,9 +3998,15 @@
       <c r="K74" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="L74" s="3"/>
-      <c r="M74" s="3"/>
-      <c r="N74" s="3"/>
+      <c r="L74" s="3" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="M74" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N74" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O74" s="2" t="n">
         <v>1</v>
       </c>
@@ -3607,9 +4045,15 @@
       <c r="K75" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="L75" s="3"/>
-      <c r="M75" s="3"/>
-      <c r="N75" s="3"/>
+      <c r="L75" s="3" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="M75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N75" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O75" s="2" t="n">
         <v>1</v>
       </c>
@@ -3648,9 +4092,15 @@
       <c r="K76" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="L76" s="3"/>
-      <c r="M76" s="3"/>
-      <c r="N76" s="3"/>
+      <c r="L76" s="3" t="n">
+        <v>11.29</v>
+      </c>
+      <c r="M76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N76" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O76" s="2" t="n">
         <v>1</v>
       </c>
@@ -3689,9 +4139,15 @@
       <c r="K77" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="L77" s="3"/>
-      <c r="M77" s="3"/>
-      <c r="N77" s="3"/>
+      <c r="L77" s="3" t="n">
+        <v>8.39</v>
+      </c>
+      <c r="M77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N77" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O77" s="2" t="n">
         <v>1</v>
       </c>
@@ -3730,9 +4186,15 @@
       <c r="K78" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
+      <c r="L78" s="3" t="n">
+        <v>0.699</v>
+      </c>
+      <c r="M78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N78" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O78" s="2" t="n">
         <v>6</v>
       </c>
@@ -3771,9 +4233,15 @@
       <c r="K79" s="2" t="n">
         <v>146</v>
       </c>
-      <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3"/>
+      <c r="L79" s="3" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="M79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N79" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O79" s="2" t="n">
         <v>5</v>
       </c>
@@ -3812,9 +4280,15 @@
       <c r="K80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="3"/>
+      <c r="L80" s="3" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="M80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N80" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O80" s="2" t="n">
         <v>2</v>
       </c>
@@ -3853,9 +4327,15 @@
       <c r="K81" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="L81" s="3"/>
-      <c r="M81" s="3"/>
-      <c r="N81" s="3"/>
+      <c r="L81" s="3" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="M81" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N81" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="O81" s="2" t="n">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
ajustes em alguns parametros do problema, para rodar o teste completo sem aproximação do resultado demora dms
</commit_message>
<xml_diff>
--- a/alimentosCompleto.xlsx
+++ b/alimentosCompleto.xlsx
@@ -314,7 +314,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -335,6 +335,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -379,7 +384,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,6 +399,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -522,7 +531,7 @@
   <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -617,10 +626,10 @@
       <c r="L2" s="3" t="n">
         <v>1.3</v>
       </c>
-      <c r="M2" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N2" s="3" t="n">
+      <c r="M2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="N2" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O2" s="2" t="n">
@@ -664,11 +673,11 @@
       <c r="L3" s="3" t="n">
         <v>2.44</v>
       </c>
-      <c r="M3" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>7</v>
+      <c r="M3" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N3" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O3" s="2" t="n">
         <v>4</v>
@@ -711,11 +720,11 @@
       <c r="L4" s="3" t="n">
         <v>6.1</v>
       </c>
-      <c r="M4" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>7</v>
+      <c r="M4" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N4" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O4" s="2" t="n">
         <v>4</v>
@@ -758,11 +767,11 @@
       <c r="L5" s="3" t="n">
         <v>1.59</v>
       </c>
-      <c r="M5" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>7</v>
+      <c r="M5" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N5" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O5" s="2" t="n">
         <v>4</v>
@@ -805,11 +814,11 @@
       <c r="L6" s="3" t="n">
         <v>0.958</v>
       </c>
-      <c r="M6" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N6" s="3" t="n">
-        <v>7</v>
+      <c r="M6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N6" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O6" s="2" t="n">
         <v>4</v>
@@ -852,11 +861,11 @@
       <c r="L7" s="3" t="n">
         <v>0.289</v>
       </c>
-      <c r="M7" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N7" s="3" t="n">
-        <v>7</v>
+      <c r="M7" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O7" s="2" t="n">
         <v>4</v>
@@ -899,11 +908,11 @@
       <c r="L8" s="3" t="n">
         <v>0.86</v>
       </c>
-      <c r="M8" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N8" s="3" t="n">
-        <v>7</v>
+      <c r="M8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="N8" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O8" s="2" t="n">
         <v>4</v>
@@ -946,11 +955,11 @@
       <c r="L9" s="3" t="n">
         <v>1.82</v>
       </c>
-      <c r="M9" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N9" s="3" t="n">
-        <v>7</v>
+      <c r="M9" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N9" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O9" s="2" t="n">
         <v>4</v>
@@ -993,11 +1002,11 @@
       <c r="L10" s="3" t="n">
         <v>6.9</v>
       </c>
-      <c r="M10" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N10" s="3" t="n">
-        <v>7</v>
+      <c r="M10" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N10" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O10" s="2" t="n">
         <v>4</v>
@@ -1040,11 +1049,11 @@
       <c r="L11" s="3" t="n">
         <v>4.99</v>
       </c>
-      <c r="M11" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N11" s="3" t="n">
-        <v>7</v>
+      <c r="M11" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N11" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O11" s="2" t="n">
         <v>4</v>
@@ -1087,11 +1096,11 @@
       <c r="L12" s="3" t="n">
         <v>1.31</v>
       </c>
-      <c r="M12" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N12" s="3" t="n">
-        <v>7</v>
+      <c r="M12" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N12" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O12" s="2" t="n">
         <v>4</v>
@@ -1134,11 +1143,11 @@
       <c r="L13" s="3" t="n">
         <v>2.27</v>
       </c>
-      <c r="M13" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N13" s="3" t="n">
-        <v>7</v>
+      <c r="M13" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="O13" s="2" t="n">
         <v>4</v>
@@ -1181,11 +1190,11 @@
       <c r="L14" s="3" t="n">
         <v>2.6</v>
       </c>
-      <c r="M14" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N14" s="3" t="n">
-        <v>7</v>
+      <c r="M14" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N14" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O14" s="2" t="n">
         <v>4</v>
@@ -1228,11 +1237,11 @@
       <c r="L15" s="3" t="n">
         <v>1.5</v>
       </c>
-      <c r="M15" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N15" s="3" t="n">
-        <v>7</v>
+      <c r="M15" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="N15" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O15" s="2" t="n">
         <v>4</v>
@@ -1275,11 +1284,11 @@
       <c r="L16" s="3" t="n">
         <v>0.699</v>
       </c>
-      <c r="M16" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N16" s="3" t="n">
-        <v>7</v>
+      <c r="M16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="N16" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O16" s="2" t="n">
         <v>4</v>
@@ -1322,11 +1331,11 @@
       <c r="L17" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="M17" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N17" s="3" t="n">
-        <v>7</v>
+      <c r="M17" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="N17" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O17" s="2" t="n">
         <v>3</v>
@@ -1369,10 +1378,10 @@
       <c r="L18" s="3" t="n">
         <v>3.75</v>
       </c>
-      <c r="M18" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N18" s="3" t="n">
+      <c r="M18" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N18" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O18" s="2" t="n">
@@ -1416,11 +1425,11 @@
       <c r="L19" s="3" t="n">
         <v>4.5</v>
       </c>
-      <c r="M19" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N19" s="3" t="n">
-        <v>7</v>
+      <c r="M19" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N19" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O19" s="2" t="n">
         <v>3</v>
@@ -1463,10 +1472,10 @@
       <c r="L20" s="3" t="n">
         <v>2.39</v>
       </c>
-      <c r="M20" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N20" s="3" t="n">
+      <c r="M20" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N20" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O20" s="2" t="n">
@@ -1510,10 +1519,10 @@
       <c r="L21" s="3" t="n">
         <v>2.49</v>
       </c>
-      <c r="M21" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N21" s="3" t="n">
+      <c r="M21" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N21" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O21" s="2" t="n">
@@ -1557,11 +1566,11 @@
       <c r="L22" s="3" t="n">
         <v>3.59</v>
       </c>
-      <c r="M22" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N22" s="3" t="n">
-        <v>7</v>
+      <c r="M22" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N22" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O22" s="2" t="n">
         <v>3</v>
@@ -1604,11 +1613,11 @@
       <c r="L23" s="3" t="n">
         <v>2.75</v>
       </c>
-      <c r="M23" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N23" s="3" t="n">
-        <v>7</v>
+      <c r="M23" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N23" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O23" s="2" t="n">
         <v>3</v>
@@ -1651,11 +1660,11 @@
       <c r="L24" s="3" t="n">
         <v>1.12</v>
       </c>
-      <c r="M24" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N24" s="3" t="n">
-        <v>7</v>
+      <c r="M24" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N24" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O24" s="2" t="n">
         <v>3</v>
@@ -1698,11 +1707,11 @@
       <c r="L25" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="M25" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N25" s="3" t="n">
-        <v>7</v>
+      <c r="M25" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N25" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O25" s="2" t="n">
         <v>3</v>
@@ -1745,11 +1754,11 @@
       <c r="L26" s="3" t="n">
         <v>1.39</v>
       </c>
-      <c r="M26" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N26" s="3" t="n">
-        <v>7</v>
+      <c r="M26" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="N26" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O26" s="2" t="n">
         <v>3</v>
@@ -1792,11 +1801,11 @@
       <c r="L27" s="3" t="n">
         <v>2.75</v>
       </c>
-      <c r="M27" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N27" s="3" t="n">
-        <v>7</v>
+      <c r="M27" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N27" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O27" s="2" t="n">
         <v>3</v>
@@ -1839,11 +1848,11 @@
       <c r="L28" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="M28" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N28" s="3" t="n">
-        <v>7</v>
+      <c r="M28" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="N28" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O28" s="2" t="n">
         <v>3</v>
@@ -1886,10 +1895,10 @@
       <c r="L29" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="M29" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N29" s="3" t="n">
+      <c r="M29" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N29" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O29" s="2" t="n">
@@ -1933,11 +1942,11 @@
       <c r="L30" s="3" t="n">
         <v>1.92</v>
       </c>
-      <c r="M30" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N30" s="3" t="n">
-        <v>7</v>
+      <c r="M30" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N30" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O30" s="2" t="n">
         <v>3</v>
@@ -1980,11 +1989,11 @@
       <c r="L31" s="3" t="n">
         <v>4.058</v>
       </c>
-      <c r="M31" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N31" s="3" t="n">
-        <v>7</v>
+      <c r="M31" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N31" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O31" s="2" t="n">
         <v>3</v>
@@ -2027,10 +2036,10 @@
       <c r="L32" s="3" t="n">
         <v>0.95</v>
       </c>
-      <c r="M32" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N32" s="3" t="n">
+      <c r="M32" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N32" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O32" s="2" t="n">
@@ -2074,11 +2083,11 @@
       <c r="L33" s="3" t="n">
         <v>2.6</v>
       </c>
-      <c r="M33" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N33" s="3" t="n">
-        <v>7</v>
+      <c r="M33" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N33" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O33" s="2" t="n">
         <v>3</v>
@@ -2121,11 +2130,11 @@
       <c r="L34" s="3" t="n">
         <v>1.5</v>
       </c>
-      <c r="M34" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N34" s="3" t="n">
-        <v>7</v>
+      <c r="M34" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N34" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O34" s="2" t="n">
         <v>3</v>
@@ -2168,11 +2177,11 @@
       <c r="L35" s="3" t="n">
         <v>4.86</v>
       </c>
-      <c r="M35" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N35" s="3" t="n">
-        <v>7</v>
+      <c r="M35" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N35" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O35" s="2" t="n">
         <v>3</v>
@@ -2215,11 +2224,11 @@
       <c r="L36" s="3" t="n">
         <v>3.21</v>
       </c>
-      <c r="M36" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N36" s="3" t="n">
-        <v>7</v>
+      <c r="M36" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N36" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O36" s="2" t="n">
         <v>3</v>
@@ -2262,11 +2271,11 @@
       <c r="L37" s="3" t="n">
         <v>3.3</v>
       </c>
-      <c r="M37" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N37" s="3" t="n">
-        <v>7</v>
+      <c r="M37" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N37" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O37" s="2" t="n">
         <v>3</v>
@@ -2309,11 +2318,11 @@
       <c r="L38" s="3" t="n">
         <v>3.12</v>
       </c>
-      <c r="M38" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N38" s="3" t="n">
-        <v>7</v>
+      <c r="M38" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N38" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O38" s="2" t="n">
         <v>3</v>
@@ -2356,11 +2365,11 @@
       <c r="L39" s="3" t="n">
         <v>1.9</v>
       </c>
-      <c r="M39" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N39" s="3" t="n">
-        <v>7</v>
+      <c r="M39" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N39" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O39" s="2" t="n">
         <v>3</v>
@@ -2403,11 +2412,11 @@
       <c r="L40" s="3" t="n">
         <v>2.79</v>
       </c>
-      <c r="M40" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N40" s="3" t="n">
-        <v>7</v>
+      <c r="M40" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N40" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O40" s="2" t="n">
         <v>3</v>
@@ -2450,10 +2459,10 @@
       <c r="L41" s="3" t="n">
         <v>5.99</v>
       </c>
-      <c r="M41" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N41" s="3" t="n">
+      <c r="M41" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N41" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O41" s="2" t="n">
@@ -2497,10 +2506,10 @@
       <c r="L42" s="3" t="n">
         <v>8.63</v>
       </c>
-      <c r="M42" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N42" s="3" t="n">
+      <c r="M42" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N42" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O42" s="2" t="n">
@@ -2544,11 +2553,11 @@
       <c r="L43" s="3" t="n">
         <v>2.2</v>
       </c>
-      <c r="M43" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N43" s="3" t="n">
-        <v>7</v>
+      <c r="M43" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N43" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O43" s="2" t="n">
         <v>3</v>
@@ -2591,10 +2600,10 @@
       <c r="L44" s="3" t="n">
         <v>1.08</v>
       </c>
-      <c r="M44" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N44" s="3" t="n">
+      <c r="M44" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="N44" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O44" s="2" t="n">
@@ -2638,11 +2647,11 @@
       <c r="L45" s="3" t="n">
         <v>2.99</v>
       </c>
-      <c r="M45" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N45" s="3" t="n">
-        <v>7</v>
+      <c r="M45" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N45" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O45" s="2" t="n">
         <v>3</v>
@@ -2685,11 +2694,11 @@
       <c r="L46" s="3" t="n">
         <v>2.9</v>
       </c>
-      <c r="M46" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N46" s="3" t="n">
-        <v>7</v>
+      <c r="M46" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N46" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O46" s="2" t="n">
         <v>2</v>
@@ -2732,11 +2741,11 @@
       <c r="L47" s="3" t="n">
         <v>1.66</v>
       </c>
-      <c r="M47" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N47" s="3" t="n">
-        <v>7</v>
+      <c r="M47" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N47" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O47" s="2" t="n">
         <v>2</v>
@@ -2779,11 +2788,11 @@
       <c r="L48" s="3" t="n">
         <v>4.98</v>
       </c>
-      <c r="M48" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N48" s="3" t="n">
-        <v>7</v>
+      <c r="M48" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N48" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O48" s="2" t="n">
         <v>2</v>
@@ -2826,11 +2835,11 @@
       <c r="L49" s="3" t="n">
         <v>1.5</v>
       </c>
-      <c r="M49" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N49" s="3" t="n">
-        <v>7</v>
+      <c r="M49" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="N49" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="O49" s="2" t="n">
         <v>2</v>
@@ -2873,11 +2882,11 @@
       <c r="L50" s="3" t="n">
         <v>1.59</v>
       </c>
-      <c r="M50" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N50" s="3" t="n">
-        <v>7</v>
+      <c r="M50" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N50" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O50" s="2" t="n">
         <v>2</v>
@@ -2920,11 +2929,11 @@
       <c r="L51" s="3" t="n">
         <v>2.29</v>
       </c>
-      <c r="M51" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N51" s="3" t="n">
-        <v>7</v>
+      <c r="M51" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N51" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O51" s="2" t="n">
         <v>2</v>
@@ -2967,11 +2976,11 @@
       <c r="L52" s="3" t="n">
         <v>3.99</v>
       </c>
-      <c r="M52" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N52" s="3" t="n">
-        <v>7</v>
+      <c r="M52" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N52" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O52" s="2" t="n">
         <v>2</v>
@@ -3014,11 +3023,11 @@
       <c r="L53" s="3" t="n">
         <v>2.1</v>
       </c>
-      <c r="M53" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N53" s="3" t="n">
-        <v>7</v>
+      <c r="M53" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N53" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="O53" s="2" t="n">
         <v>2</v>
@@ -3061,11 +3070,11 @@
       <c r="L54" s="3" t="n">
         <v>8.5</v>
       </c>
-      <c r="M54" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N54" s="3" t="n">
-        <v>7</v>
+      <c r="M54" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N54" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O54" s="2" t="n">
         <v>2</v>
@@ -3108,11 +3117,11 @@
       <c r="L55" s="3" t="n">
         <v>1.7</v>
       </c>
-      <c r="M55" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N55" s="3" t="n">
-        <v>7</v>
+      <c r="M55" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N55" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O55" s="2" t="n">
         <v>2</v>
@@ -3155,10 +3164,10 @@
       <c r="L56" s="3" t="n">
         <v>1.69</v>
       </c>
-      <c r="M56" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N56" s="3" t="n">
+      <c r="M56" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N56" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O56" s="2" t="n">
@@ -3202,10 +3211,10 @@
       <c r="L57" s="3" t="n">
         <v>0.298</v>
       </c>
-      <c r="M57" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N57" s="3" t="n">
+      <c r="M57" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N57" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O57" s="2" t="n">
@@ -3249,10 +3258,10 @@
       <c r="L58" s="3" t="n">
         <v>1.99</v>
       </c>
-      <c r="M58" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N58" s="3" t="n">
+      <c r="M58" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N58" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O58" s="2" t="n">
@@ -3296,11 +3305,11 @@
       <c r="L59" s="3" t="n">
         <v>1.19</v>
       </c>
-      <c r="M59" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N59" s="3" t="n">
-        <v>7</v>
+      <c r="M59" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N59" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O59" s="2" t="n">
         <v>2</v>
@@ -3343,11 +3352,11 @@
       <c r="L60" s="3" t="n">
         <v>0.99</v>
       </c>
-      <c r="M60" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N60" s="3" t="n">
-        <v>7</v>
+      <c r="M60" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N60" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O60" s="2" t="n">
         <v>2</v>
@@ -3390,11 +3399,11 @@
       <c r="L61" s="3" t="n">
         <v>2.268</v>
       </c>
-      <c r="M61" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N61" s="3" t="n">
-        <v>7</v>
+      <c r="M61" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N61" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="O61" s="2" t="n">
         <v>2</v>
@@ -3437,11 +3446,11 @@
       <c r="L62" s="3" t="n">
         <v>0.299</v>
       </c>
-      <c r="M62" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N62" s="3" t="n">
-        <v>7</v>
+      <c r="M62" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N62" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O62" s="2" t="n">
         <v>2</v>
@@ -3484,11 +3493,11 @@
       <c r="L63" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="M63" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N63" s="3" t="n">
-        <v>7</v>
+      <c r="M63" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N63" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O63" s="2" t="n">
         <v>2</v>
@@ -3531,11 +3540,11 @@
       <c r="L64" s="3" t="n">
         <v>0.99</v>
       </c>
-      <c r="M64" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N64" s="3" t="n">
-        <v>7</v>
+      <c r="M64" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N64" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O64" s="2" t="n">
         <v>2</v>
@@ -3578,11 +3587,11 @@
       <c r="L65" s="3" t="n">
         <v>5.2</v>
       </c>
-      <c r="M65" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N65" s="3" t="n">
-        <v>7</v>
+      <c r="M65" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N65" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O65" s="2" t="n">
         <v>2</v>
@@ -3625,11 +3634,11 @@
       <c r="L66" s="3" t="n">
         <v>15.9</v>
       </c>
-      <c r="M66" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N66" s="3" t="n">
-        <v>7</v>
+      <c r="M66" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="N66" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="O66" s="2" t="n">
         <v>2</v>
@@ -3672,11 +3681,11 @@
       <c r="L67" s="3" t="n">
         <v>1.49</v>
       </c>
-      <c r="M67" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N67" s="3" t="n">
-        <v>7</v>
+      <c r="M67" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N67" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O67" s="2" t="n">
         <v>2</v>
@@ -3719,11 +3728,11 @@
       <c r="L68" s="3" t="n">
         <v>3.1</v>
       </c>
-      <c r="M68" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N68" s="3" t="n">
-        <v>7</v>
+      <c r="M68" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N68" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O68" s="2" t="n">
         <v>2</v>
@@ -3766,11 +3775,11 @@
       <c r="L69" s="3" t="n">
         <v>0.99</v>
       </c>
-      <c r="M69" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N69" s="3" t="n">
-        <v>7</v>
+      <c r="M69" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N69" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O69" s="2" t="n">
         <v>2</v>
@@ -3813,11 +3822,11 @@
       <c r="L70" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="M70" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N70" s="3" t="n">
-        <v>7</v>
+      <c r="M70" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N70" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="O70" s="2" t="n">
         <v>2</v>
@@ -3860,11 +3869,11 @@
       <c r="L71" s="3" t="n">
         <v>2.67</v>
       </c>
-      <c r="M71" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N71" s="3" t="n">
-        <v>7</v>
+      <c r="M71" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="N71" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O71" s="2" t="n">
         <v>1</v>
@@ -3907,11 +3916,11 @@
       <c r="L72" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="M72" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N72" s="3" t="n">
-        <v>7</v>
+      <c r="M72" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N72" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="O72" s="2" t="n">
         <v>1</v>
@@ -3954,11 +3963,11 @@
       <c r="L73" s="3" t="n">
         <v>2.179</v>
       </c>
-      <c r="M73" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N73" s="3" t="n">
-        <v>7</v>
+      <c r="M73" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N73" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="O73" s="2" t="n">
         <v>1</v>
@@ -4001,11 +4010,11 @@
       <c r="L74" s="3" t="n">
         <v>0.49</v>
       </c>
-      <c r="M74" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N74" s="3" t="n">
-        <v>7</v>
+      <c r="M74" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N74" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="O74" s="2" t="n">
         <v>1</v>
@@ -4048,11 +4057,11 @@
       <c r="L75" s="3" t="n">
         <v>5.99</v>
       </c>
-      <c r="M75" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N75" s="3" t="n">
-        <v>7</v>
+      <c r="M75" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="N75" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O75" s="2" t="n">
         <v>1</v>
@@ -4095,11 +4104,11 @@
       <c r="L76" s="3" t="n">
         <v>11.29</v>
       </c>
-      <c r="M76" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N76" s="3" t="n">
-        <v>7</v>
+      <c r="M76" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="N76" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="O76" s="2" t="n">
         <v>1</v>
@@ -4142,11 +4151,11 @@
       <c r="L77" s="3" t="n">
         <v>8.39</v>
       </c>
-      <c r="M77" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N77" s="3" t="n">
-        <v>7</v>
+      <c r="M77" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N77" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="O77" s="2" t="n">
         <v>1</v>
@@ -4189,10 +4198,10 @@
       <c r="L78" s="3" t="n">
         <v>0.699</v>
       </c>
-      <c r="M78" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N78" s="3" t="n">
+      <c r="M78" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="N78" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O78" s="2" t="n">
@@ -4236,10 +4245,10 @@
       <c r="L79" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="M79" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N79" s="3" t="n">
+      <c r="M79" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="N79" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O79" s="2" t="n">
@@ -4283,10 +4292,10 @@
       <c r="L80" s="3" t="n">
         <v>1.65</v>
       </c>
-      <c r="M80" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N80" s="3" t="n">
+      <c r="M80" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N80" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O80" s="2" t="n">
@@ -4330,10 +4339,10 @@
       <c r="L81" s="3" t="n">
         <v>2.49</v>
       </c>
-      <c r="M81" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="N81" s="3" t="n">
+      <c r="M81" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="N81" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O81" s="2" t="n">

</xml_diff>

<commit_message>
adicão de mais alguns alimentos, percebi que quanto menos dias max por alimento o modelo demora bem mais. Talvez seja interessante usar o gap por enqt ta 5%
</commit_message>
<xml_diff>
--- a/alimentosCompleto.xlsx
+++ b/alimentosCompleto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -274,6 +274,9 @@
     <t xml:space="preserve">uva</t>
   </si>
   <si>
+    <t xml:space="preserve">banana</t>
+  </si>
+  <si>
     <t xml:space="preserve">achocolatado</t>
   </si>
   <si>
@@ -298,13 +301,25 @@
     <t xml:space="preserve">feijao</t>
   </si>
   <si>
+    <t xml:space="preserve">amendoim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carne</t>
+  </si>
+  <si>
     <t xml:space="preserve">ovo</t>
   </si>
   <si>
-    <t xml:space="preserve">banana</t>
-  </si>
-  <si>
     <t xml:space="preserve">frango</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">azeite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manteiga</t>
   </si>
 </sst>
 </file>
@@ -340,6 +355,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -401,7 +417,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -528,10 +544,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O81"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="Q7" activeCellId="0" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -677,7 +695,7 @@
         <v>10</v>
       </c>
       <c r="N3" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O3" s="2" t="n">
         <v>4</v>
@@ -724,7 +742,7 @@
         <v>8</v>
       </c>
       <c r="N4" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O4" s="2" t="n">
         <v>4</v>
@@ -771,7 +789,7 @@
         <v>8</v>
       </c>
       <c r="N5" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O5" s="2" t="n">
         <v>4</v>
@@ -818,7 +836,7 @@
         <v>8</v>
       </c>
       <c r="N6" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O6" s="2" t="n">
         <v>4</v>
@@ -865,7 +883,7 @@
         <v>10</v>
       </c>
       <c r="N7" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O7" s="2" t="n">
         <v>4</v>
@@ -912,7 +930,7 @@
         <v>15</v>
       </c>
       <c r="N8" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O8" s="2" t="n">
         <v>4</v>
@@ -959,7 +977,7 @@
         <v>10</v>
       </c>
       <c r="N9" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O9" s="2" t="n">
         <v>4</v>
@@ -1006,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="N10" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O10" s="2" t="n">
         <v>4</v>
@@ -1053,7 +1071,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O11" s="2" t="n">
         <v>4</v>
@@ -1100,7 +1118,7 @@
         <v>5</v>
       </c>
       <c r="N12" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O12" s="2" t="n">
         <v>4</v>
@@ -1147,7 +1165,7 @@
         <v>5</v>
       </c>
       <c r="N13" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O13" s="2" t="n">
         <v>4</v>
@@ -1194,7 +1212,7 @@
         <v>10</v>
       </c>
       <c r="N14" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O14" s="2" t="n">
         <v>4</v>
@@ -1241,7 +1259,7 @@
         <v>15</v>
       </c>
       <c r="N15" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O15" s="2" t="n">
         <v>4</v>
@@ -1288,7 +1306,7 @@
         <v>15</v>
       </c>
       <c r="N16" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O16" s="2" t="n">
         <v>4</v>
@@ -1335,7 +1353,7 @@
         <v>12</v>
       </c>
       <c r="N17" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O17" s="2" t="n">
         <v>3</v>
@@ -1429,7 +1447,7 @@
         <v>10</v>
       </c>
       <c r="N19" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O19" s="2" t="n">
         <v>3</v>
@@ -1570,7 +1588,7 @@
         <v>8</v>
       </c>
       <c r="N22" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O22" s="2" t="n">
         <v>3</v>
@@ -1617,7 +1635,7 @@
         <v>10</v>
       </c>
       <c r="N23" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O23" s="2" t="n">
         <v>3</v>
@@ -1664,7 +1682,7 @@
         <v>10</v>
       </c>
       <c r="N24" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O24" s="2" t="n">
         <v>3</v>
@@ -1711,7 +1729,7 @@
         <v>10</v>
       </c>
       <c r="N25" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O25" s="2" t="n">
         <v>3</v>
@@ -1758,7 +1776,7 @@
         <v>12</v>
       </c>
       <c r="N26" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O26" s="2" t="n">
         <v>3</v>
@@ -1805,7 +1823,7 @@
         <v>8</v>
       </c>
       <c r="N27" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O27" s="2" t="n">
         <v>3</v>
@@ -1852,7 +1870,7 @@
         <v>12</v>
       </c>
       <c r="N28" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O28" s="2" t="n">
         <v>3</v>
@@ -1946,7 +1964,7 @@
         <v>10</v>
       </c>
       <c r="N30" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O30" s="2" t="n">
         <v>3</v>
@@ -1993,7 +2011,7 @@
         <v>8</v>
       </c>
       <c r="N31" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O31" s="2" t="n">
         <v>3</v>
@@ -2087,7 +2105,7 @@
         <v>8</v>
       </c>
       <c r="N33" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O33" s="2" t="n">
         <v>3</v>
@@ -2134,7 +2152,7 @@
         <v>8</v>
       </c>
       <c r="N34" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O34" s="2" t="n">
         <v>3</v>
@@ -2181,7 +2199,7 @@
         <v>8</v>
       </c>
       <c r="N35" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O35" s="2" t="n">
         <v>3</v>
@@ -2228,7 +2246,7 @@
         <v>5</v>
       </c>
       <c r="N36" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O36" s="2" t="n">
         <v>3</v>
@@ -2275,7 +2293,7 @@
         <v>10</v>
       </c>
       <c r="N37" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O37" s="2" t="n">
         <v>3</v>
@@ -2322,7 +2340,7 @@
         <v>8</v>
       </c>
       <c r="N38" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O38" s="2" t="n">
         <v>3</v>
@@ -2369,7 +2387,7 @@
         <v>10</v>
       </c>
       <c r="N39" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O39" s="2" t="n">
         <v>3</v>
@@ -2416,7 +2434,7 @@
         <v>10</v>
       </c>
       <c r="N40" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O40" s="2" t="n">
         <v>3</v>
@@ -2557,7 +2575,7 @@
         <v>8</v>
       </c>
       <c r="N43" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O43" s="2" t="n">
         <v>3</v>
@@ -2651,7 +2669,7 @@
         <v>10</v>
       </c>
       <c r="N45" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O45" s="2" t="n">
         <v>3</v>
@@ -2698,7 +2716,7 @@
         <v>5</v>
       </c>
       <c r="N46" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O46" s="2" t="n">
         <v>2</v>
@@ -2745,7 +2763,7 @@
         <v>5</v>
       </c>
       <c r="N47" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O47" s="2" t="n">
         <v>2</v>
@@ -2792,7 +2810,7 @@
         <v>5</v>
       </c>
       <c r="N48" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O48" s="2" t="n">
         <v>2</v>
@@ -2839,7 +2857,7 @@
         <v>4</v>
       </c>
       <c r="N49" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O49" s="2" t="n">
         <v>2</v>
@@ -2886,7 +2904,7 @@
         <v>8</v>
       </c>
       <c r="N50" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O50" s="2" t="n">
         <v>2</v>
@@ -2933,7 +2951,7 @@
         <v>5</v>
       </c>
       <c r="N51" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O51" s="2" t="n">
         <v>2</v>
@@ -2980,7 +2998,7 @@
         <v>5</v>
       </c>
       <c r="N52" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O52" s="2" t="n">
         <v>2</v>
@@ -3027,7 +3045,7 @@
         <v>5</v>
       </c>
       <c r="N53" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O53" s="2" t="n">
         <v>2</v>
@@ -3074,7 +3092,7 @@
         <v>5</v>
       </c>
       <c r="N54" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O54" s="2" t="n">
         <v>2</v>
@@ -3121,7 +3139,7 @@
         <v>5</v>
       </c>
       <c r="N55" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O55" s="2" t="n">
         <v>2</v>
@@ -3309,7 +3327,7 @@
         <v>8</v>
       </c>
       <c r="N59" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O59" s="2" t="n">
         <v>2</v>
@@ -3356,7 +3374,7 @@
         <v>8</v>
       </c>
       <c r="N60" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O60" s="2" t="n">
         <v>2</v>
@@ -3403,7 +3421,7 @@
         <v>5</v>
       </c>
       <c r="N61" s="4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O61" s="2" t="n">
         <v>2</v>
@@ -3450,7 +3468,7 @@
         <v>8</v>
       </c>
       <c r="N62" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O62" s="2" t="n">
         <v>2</v>
@@ -3497,7 +3515,7 @@
         <v>8</v>
       </c>
       <c r="N63" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O63" s="2" t="n">
         <v>2</v>
@@ -3544,7 +3562,7 @@
         <v>8</v>
       </c>
       <c r="N64" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O64" s="2" t="n">
         <v>2</v>
@@ -3591,7 +3609,7 @@
         <v>8</v>
       </c>
       <c r="N65" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O65" s="2" t="n">
         <v>2</v>
@@ -3638,7 +3656,7 @@
         <v>4</v>
       </c>
       <c r="N66" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O66" s="2" t="n">
         <v>2</v>
@@ -3685,7 +3703,7 @@
         <v>8</v>
       </c>
       <c r="N67" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O67" s="2" t="n">
         <v>2</v>
@@ -3732,7 +3750,7 @@
         <v>8</v>
       </c>
       <c r="N68" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O68" s="2" t="n">
         <v>2</v>
@@ -3779,7 +3797,7 @@
         <v>8</v>
       </c>
       <c r="N69" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O69" s="2" t="n">
         <v>2</v>
@@ -3826,7 +3844,7 @@
         <v>8</v>
       </c>
       <c r="N70" s="4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O70" s="2" t="n">
         <v>2</v>
@@ -3834,93 +3852,93 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
-        <v>491</v>
+        <v>175</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>401</v>
+        <v>128</v>
       </c>
       <c r="D71" s="2" t="n">
-        <v>91.2</v>
+        <v>33.7</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>4.2</v>
+        <v>1.4</v>
       </c>
       <c r="F71" s="2" t="n">
-        <v>2.2</v>
+        <v>0.2</v>
       </c>
       <c r="G71" s="2" t="n">
-        <v>5.4</v>
+        <v>0.3</v>
       </c>
       <c r="H71" s="2" t="n">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="I71" s="2" t="n">
-        <v>0</v>
+        <v>15.7</v>
       </c>
       <c r="J71" s="2" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="K71" s="2" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="L71" s="3" t="n">
-        <v>2.67</v>
+        <v>1.65</v>
       </c>
       <c r="M71" s="4" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N71" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O71" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>99.6</v>
+        <v>91.2</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>0.3</v>
+        <v>4.2</v>
       </c>
       <c r="F72" s="2" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="G72" s="2" t="n">
-        <v>0.2</v>
+        <v>5.4</v>
       </c>
       <c r="H72" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="I72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I72" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J72" s="2" t="n">
-        <v>0</v>
-      </c>
       <c r="K72" s="2" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="L72" s="3" t="n">
-        <v>0.5</v>
+        <v>2.67</v>
       </c>
       <c r="M72" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N72" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O72" s="2" t="n">
         <v>1</v>
@@ -3928,46 +3946,46 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>369</v>
+        <v>387</v>
       </c>
       <c r="D73" s="2" t="n">
-        <v>94.5</v>
+        <v>99.6</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="F73" s="2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G73" s="2" t="n">
-        <v>8.3</v>
+        <v>0.2</v>
       </c>
       <c r="H73" s="2" t="n">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="I73" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L73" s="3" t="n">
         <v>0.5</v>
-      </c>
-      <c r="K73" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="L73" s="3" t="n">
-        <v>2.179</v>
       </c>
       <c r="M73" s="4" t="n">
         <v>3</v>
       </c>
       <c r="N73" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O73" s="2" t="n">
         <v>1</v>
@@ -3975,46 +3993,46 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="D74" s="2" t="n">
-        <v>99.5</v>
+        <v>94.5</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="F74" s="2" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G74" s="2" t="n">
-        <v>0.1</v>
+        <v>8.3</v>
       </c>
       <c r="H74" s="2" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="I74" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J74" s="2" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K74" s="2" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="L74" s="3" t="n">
-        <v>0.49</v>
+        <v>2.179</v>
       </c>
       <c r="M74" s="4" t="n">
         <v>3</v>
       </c>
       <c r="N74" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O74" s="2" t="n">
         <v>1</v>
@@ -4022,46 +4040,46 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>540</v>
+        <v>387</v>
       </c>
       <c r="D75" s="2" t="n">
-        <v>59.6</v>
+        <v>99.5</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>7.2</v>
+        <v>0.3</v>
       </c>
       <c r="F75" s="2" t="n">
-        <v>30.3</v>
+        <v>0</v>
       </c>
       <c r="G75" s="2" t="n">
-        <v>1.6</v>
+        <v>0.1</v>
       </c>
       <c r="H75" s="2" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="I75" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J75" s="2" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="K75" s="2" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="L75" s="3" t="n">
-        <v>5.99</v>
+        <v>0.49</v>
       </c>
       <c r="M75" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N75" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O75" s="2" t="n">
         <v>1</v>
@@ -4069,46 +4087,46 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>475</v>
+        <v>540</v>
       </c>
       <c r="D76" s="2" t="n">
-        <v>62.4</v>
+        <v>59.6</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>4.9</v>
+        <v>7.2</v>
       </c>
       <c r="F76" s="2" t="n">
-        <v>29.9</v>
+        <v>30.3</v>
       </c>
       <c r="G76" s="2" t="n">
-        <v>3.6</v>
+        <v>1.6</v>
       </c>
       <c r="H76" s="2" t="n">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="I76" s="2" t="n">
-        <v>2.1</v>
+        <v>0</v>
       </c>
       <c r="J76" s="2" t="n">
-        <v>1.5</v>
+        <v>1.1</v>
       </c>
       <c r="K76" s="2" t="n">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="L76" s="3" t="n">
-        <v>11.29</v>
+        <v>5.99</v>
       </c>
       <c r="M76" s="4" t="n">
         <v>4</v>
       </c>
       <c r="N76" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O76" s="2" t="n">
         <v>1</v>
@@ -4116,46 +4134,46 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>449</v>
+        <v>475</v>
       </c>
       <c r="D77" s="2" t="n">
-        <v>81.4</v>
+        <v>62.4</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>1.1</v>
+        <v>4.9</v>
       </c>
       <c r="F77" s="2" t="n">
-        <v>13.6</v>
+        <v>29.9</v>
       </c>
       <c r="G77" s="2" t="n">
-        <v>1.2</v>
+        <v>3.6</v>
       </c>
       <c r="H77" s="2" t="n">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="I77" s="2" t="n">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="J77" s="2" t="n">
-        <v>0.4</v>
+        <v>1.5</v>
       </c>
       <c r="K77" s="2" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="L77" s="3" t="n">
-        <v>8.39</v>
+        <v>11.29</v>
       </c>
       <c r="M77" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N77" s="4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O77" s="2" t="n">
         <v>1</v>
@@ -4163,181 +4181,181 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
-        <v>561</v>
+        <v>499</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>76</v>
+        <v>449</v>
       </c>
       <c r="D78" s="2" t="n">
+        <v>81.4</v>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="F78" s="2" t="n">
         <v>13.6</v>
       </c>
-      <c r="E78" s="2" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="F78" s="2" t="n">
-        <v>0.5</v>
-      </c>
       <c r="G78" s="2" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="H78" s="2" t="n">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="I78" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J78" s="2" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K78" s="2" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="L78" s="3" t="n">
-        <v>0.699</v>
+        <v>8.39</v>
       </c>
       <c r="M78" s="4" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="N78" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O78" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
-        <v>488</v>
+        <v>561</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C79" s="2" t="n">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="D79" s="2" t="n">
-        <v>0.6</v>
+        <v>13.6</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>13.3</v>
+        <v>4.8</v>
       </c>
       <c r="F79" s="2" t="n">
-        <v>9.5</v>
+        <v>0.5</v>
       </c>
       <c r="G79" s="2" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="H79" s="2" t="n">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="I79" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J79" s="2" t="n">
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
       <c r="K79" s="2" t="n">
-        <v>146</v>
+        <v>2</v>
       </c>
       <c r="L79" s="3" t="n">
-        <v>1.8</v>
+        <v>0.699</v>
       </c>
       <c r="M79" s="4" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="N79" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O79" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
-        <v>175</v>
+        <v>558</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C80" s="2" t="n">
-        <v>128</v>
+        <v>606</v>
       </c>
       <c r="D80" s="2" t="n">
-        <v>33.7</v>
+        <v>18.7</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>1.4</v>
+        <v>22.5</v>
       </c>
       <c r="F80" s="2" t="n">
-        <v>0.2</v>
+        <v>54</v>
       </c>
       <c r="G80" s="2" t="n">
-        <v>0.3</v>
+        <v>1.3</v>
       </c>
       <c r="H80" s="2" t="n">
-        <v>24</v>
+        <v>159</v>
       </c>
       <c r="I80" s="2" t="n">
-        <v>15.7</v>
+        <v>0</v>
       </c>
       <c r="J80" s="2" t="n">
-        <v>0.2</v>
+        <v>2.1</v>
       </c>
       <c r="K80" s="2" t="n">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="L80" s="3" t="n">
-        <v>1.65</v>
+        <v>3.89</v>
       </c>
       <c r="M80" s="4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N80" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O80" s="2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
-        <v>406</v>
+        <v>377</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C81" s="2" t="n">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D81" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>33.4</v>
+        <v>35.9</v>
       </c>
       <c r="F81" s="2" t="n">
-        <v>7.6</v>
+        <v>7.3</v>
       </c>
       <c r="G81" s="2" t="n">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="H81" s="2" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I81" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J81" s="2" t="n">
-        <v>1</v>
+        <v>8.1</v>
       </c>
       <c r="K81" s="2" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L81" s="3" t="n">
-        <v>2.49</v>
+        <v>5.69</v>
       </c>
       <c r="M81" s="4" t="n">
         <v>20</v>
@@ -4347,6 +4365,241 @@
       </c>
       <c r="O81" s="2" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="n">
+        <v>488</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>146</v>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F82" s="2" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G82" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H82" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="I82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K82" s="2" t="n">
+        <v>146</v>
+      </c>
+      <c r="L82" s="3" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="M82" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="N82" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O82" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="n">
+        <v>406</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="2" t="n">
+        <v>212</v>
+      </c>
+      <c r="D83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="F83" s="2" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="G83" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H83" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="I83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K83" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="L83" s="3" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="M83" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="N83" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O83" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="n">
+        <v>277</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" s="2" t="n">
+        <v>166</v>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="F84" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G84" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="H84" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="I84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K84" s="2" t="n">
+        <v>362</v>
+      </c>
+      <c r="L84" s="3" t="n">
+        <v>5.35</v>
+      </c>
+      <c r="M84" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N84" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O84" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>884</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" s="1" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="M85" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N85" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O85" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>726</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>82.4</v>
+      </c>
+      <c r="G86" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K86" s="0" t="n">
+        <v>579</v>
+      </c>
+      <c r="L86" s="1" t="n">
+        <v>6.49</v>
+      </c>
+      <c r="M86" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N86" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O86" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mudanças nos logs, ajustes finais do modelo
</commit_message>
<xml_diff>
--- a/alimentosCompleto.xlsx
+++ b/alimentosCompleto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -73,18 +73,6 @@
     <t xml:space="preserve">aveia</t>
   </si>
   <si>
-    <t xml:space="preserve">farinhaDeArroz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farinhaDeCenteio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farinhaDeMilho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farinhaDeTrigo</t>
-  </si>
-  <si>
     <t xml:space="preserve">macarrão</t>
   </si>
   <si>
@@ -278,15 +266,6 @@
   </si>
   <si>
     <t xml:space="preserve">achocolatado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acucarCristal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acucarMascavo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acucarRefinado</t>
   </si>
   <si>
     <t xml:space="preserve">chocolateAoLeite</t>
@@ -544,12 +523,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O86"/>
+  <dimension ref="A1:O79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="Q7" activeCellId="0" sqref="Q7"/>
+      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,46 +682,46 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>85.5</v>
+        <v>77.9</v>
       </c>
       <c r="E4" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>1.3</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>0.3</v>
-      </c>
       <c r="G4" s="2" t="n">
-        <v>31.4</v>
+        <v>0.9</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>173.6</v>
+        <v>0</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>8.5</v>
+        <v>0.8</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>6.1</v>
+        <v>0.86</v>
       </c>
       <c r="M4" s="4" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N4" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O4" s="2" t="n">
         <v>4</v>
@@ -750,46 +729,46 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>336</v>
+        <v>361</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>73.3</v>
+        <v>87.1</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>12.5</v>
+        <v>0.6</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>4.7</v>
+        <v>0.1</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>2.7</v>
+        <v>0.1</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>1.59</v>
+        <v>1.82</v>
       </c>
       <c r="M5" s="4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N5" s="4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O5" s="2" t="n">
         <v>4</v>
@@ -797,28 +776,28 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>351</v>
+        <v>370</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>79.1</v>
+        <v>80.8</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>2.3</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>0</v>
@@ -827,16 +806,16 @@
         <v>0.6</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>45</v>
+        <v>272</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>0.958</v>
+        <v>6.9</v>
       </c>
       <c r="M6" s="4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N6" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O6" s="2" t="n">
         <v>4</v>
@@ -844,43 +823,43 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>360</v>
+        <v>386</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>75.1</v>
+        <v>83.9</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>9.8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0.8</v>
+        <v>1.9</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>0.289</v>
+        <v>4.99</v>
       </c>
       <c r="M7" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N7" s="4" t="n">
         <v>1</v>
@@ -891,46 +870,46 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>371</v>
+        <v>333</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>77.9</v>
+        <v>86.1</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>10</v>
+        <v>4.8</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>0.9</v>
+        <v>4.3</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0</v>
+        <v>96.3</v>
       </c>
       <c r="J8" s="2" t="n">
         <v>0.8</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>7</v>
+        <v>594</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>0.86</v>
+        <v>1.31</v>
       </c>
       <c r="M8" s="4" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="N8" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O8" s="2" t="n">
         <v>4</v>
@@ -938,46 +917,46 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>87.1</v>
+        <v>78.1</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0.6</v>
+        <v>7.2</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>1.82</v>
+        <v>2.27</v>
       </c>
       <c r="M9" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N9" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O9" s="2" t="n">
         <v>4</v>
@@ -985,46 +964,46 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>370</v>
+        <v>80</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>80.8</v>
+        <v>18.9</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>7.3</v>
+        <v>0.9</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>1.6</v>
+        <v>0.2</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0</v>
+        <v>17.1</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>272</v>
+        <v>2</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>6.9</v>
+        <v>2.6</v>
       </c>
       <c r="M10" s="4" t="n">
         <v>10</v>
       </c>
       <c r="N10" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O10" s="2" t="n">
         <v>4</v>
@@ -1032,46 +1011,46 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>386</v>
+        <v>77</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>83.9</v>
+        <v>18.4</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>7</v>
+        <v>0.6</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0</v>
+        <v>23.8</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>1.9</v>
+        <v>0.1</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>4.99</v>
+        <v>1.5</v>
       </c>
       <c r="M11" s="4" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N11" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O11" s="2" t="n">
         <v>4</v>
@@ -1079,46 +1058,46 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>333</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>86.1</v>
+        <v>11.9</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>4.8</v>
+        <v>1.2</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>4.3</v>
+        <v>0.2</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>96.3</v>
+        <v>3.8</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>594</v>
+        <v>2</v>
       </c>
       <c r="L12" s="3" t="n">
-        <v>1.31</v>
+        <v>0.699</v>
       </c>
       <c r="M12" s="4" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N12" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O12" s="2" t="n">
         <v>4</v>
@@ -1126,87 +1105,87 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>358</v>
+        <v>48</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>78.1</v>
+        <v>10.8</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>7.2</v>
+        <v>1.4</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>0.3</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>2.27</v>
+        <v>0.4</v>
       </c>
       <c r="M13" s="4" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="N13" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O13" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>18.9</v>
+        <v>2.3</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0.9</v>
+        <v>2.7</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>0.4</v>
+        <v>3.1</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>17.1</v>
+        <v>60.1</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>2.6</v>
+        <v>3.75</v>
       </c>
       <c r="M14" s="4" t="n">
         <v>10</v>
@@ -1215,145 +1194,145 @@
         <v>7</v>
       </c>
       <c r="O14" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>18.4</v>
+        <v>4.3</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>23.8</v>
+        <v>5.9</v>
       </c>
       <c r="J15" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="M15" s="4" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N15" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O15" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>11.9</v>
+        <v>2.5</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>0.2</v>
+        <v>2.5</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>3.8</v>
+        <v>13.5</v>
       </c>
       <c r="J16" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L16" s="3" t="n">
-        <v>0.699</v>
+        <v>2.39</v>
       </c>
       <c r="M16" s="4" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N16" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O16" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>10.8</v>
+        <v>23.9</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>1.4</v>
+        <v>7</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L17" s="3" t="n">
-        <v>0.4</v>
+        <v>2.49</v>
       </c>
       <c r="M17" s="4" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="N17" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O17" s="2" t="n">
         <v>3</v>
@@ -1361,46 +1340,46 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>2.3</v>
+        <v>6.9</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>2.7</v>
+        <v>1.4</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>3.1</v>
+        <v>0.6</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>60.1</v>
+        <v>14.1</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L18" s="3" t="n">
-        <v>3.75</v>
+        <v>3.59</v>
       </c>
       <c r="M18" s="4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N18" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O18" s="2" t="n">
         <v>3</v>
@@ -1408,46 +1387,46 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>4.3</v>
+        <v>3.3</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>0.7</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>5.9</v>
+        <v>1.7</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L19" s="3" t="n">
-        <v>4.5</v>
+        <v>2.75</v>
       </c>
       <c r="M19" s="4" t="n">
         <v>10</v>
       </c>
       <c r="N19" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O19" s="2" t="n">
         <v>3</v>
@@ -1455,46 +1434,46 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>2.5</v>
+        <v>0.2</v>
       </c>
       <c r="H20" s="2" t="n">
         <v>9</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>13.5</v>
+        <v>0</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>2.39</v>
+        <v>1.12</v>
       </c>
       <c r="M20" s="4" t="n">
         <v>10</v>
       </c>
       <c r="N20" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O20" s="2" t="n">
         <v>3</v>
@@ -1502,46 +1481,46 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>113</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>23.9</v>
+        <v>7.2</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>7</v>
+        <v>1.3</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="L21" s="3" t="n">
-        <v>2.49</v>
+        <v>0.5</v>
       </c>
       <c r="M21" s="4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N21" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O21" s="2" t="n">
         <v>3</v>
@@ -1549,46 +1528,46 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>6.9</v>
+        <v>23.2</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>14.1</v>
+        <v>5.6</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="K22" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L22" s="3" t="n">
-        <v>3.59</v>
+        <v>1.39</v>
       </c>
       <c r="M22" s="4" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N22" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O22" s="2" t="n">
         <v>3</v>
@@ -1596,46 +1575,46 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>3.3</v>
+        <v>6.2</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H23" s="2" t="n">
         <v>21</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>1.7</v>
+        <v>6.8</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="K23" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L23" s="3" t="n">
         <v>2.75</v>
       </c>
       <c r="M23" s="4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N23" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O23" s="2" t="n">
         <v>3</v>
@@ -1643,46 +1622,46 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>19</v>
+        <v>151</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>4.5</v>
+        <v>36.2</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.7</v>
+        <v>1.1</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="J24" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K24" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L24" s="3" t="n">
-        <v>1.12</v>
+        <v>0.5</v>
       </c>
       <c r="M24" s="4" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N24" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O24" s="2" t="n">
         <v>3</v>
@@ -1690,46 +1669,46 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>7.2</v>
+        <v>3.6</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>1.2</v>
+        <v>2.3</v>
       </c>
       <c r="J25" s="2" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="K25" s="2" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="L25" s="3" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="M25" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N25" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O25" s="2" t="n">
         <v>3</v>
@@ -1737,16 +1716,16 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>23.2</v>
+        <v>3.2</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>2.1</v>
@@ -1755,28 +1734,28 @@
         <v>0.2</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>0.4</v>
+        <v>1.1</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>5.6</v>
+        <v>38.6</v>
       </c>
       <c r="J26" s="2" t="n">
         <v>0.3</v>
       </c>
       <c r="K26" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L26" s="3" t="n">
-        <v>1.39</v>
+        <v>1.92</v>
       </c>
       <c r="M26" s="4" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N26" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O26" s="2" t="n">
         <v>3</v>
@@ -1784,46 +1763,46 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>6.2</v>
+        <v>5.5</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>1.4</v>
+        <v>2.5</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>6.8</v>
+        <v>8.7</v>
       </c>
       <c r="J27" s="2" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="K27" s="2" t="n">
-        <v>0</v>
+        <v>563</v>
       </c>
       <c r="L27" s="3" t="n">
-        <v>2.75</v>
+        <v>4.058</v>
       </c>
       <c r="M27" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N27" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O27" s="2" t="n">
         <v>3</v>
@@ -1831,46 +1810,46 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>36.2</v>
+        <v>2</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>1.1</v>
+        <v>0.9</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>16.5</v>
+        <v>5</v>
       </c>
       <c r="J28" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K28" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L28" s="3" t="n">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="M28" s="4" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N28" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O28" s="2" t="n">
         <v>3</v>
@@ -1878,46 +1857,46 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>3.6</v>
+        <v>6</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="I29" s="2" t="n">
-        <v>2.3</v>
+        <v>201.4</v>
       </c>
       <c r="J29" s="2" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="K29" s="2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L29" s="3" t="n">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="M29" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N29" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O29" s="2" t="n">
         <v>3</v>
@@ -1925,46 +1904,46 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>3.2</v>
+        <v>4.9</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>2.1</v>
+        <v>1.1</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>1.1</v>
+        <v>0.4</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>38.6</v>
+        <v>100.2</v>
       </c>
       <c r="J30" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="K30" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L30" s="3" t="n">
-        <v>1.92</v>
+        <v>1.5</v>
       </c>
       <c r="M30" s="4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N30" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O30" s="2" t="n">
         <v>3</v>
@@ -1972,46 +1951,46 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D31" s="2" t="n">
         <v>5.5</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>8.7</v>
+        <v>158.2</v>
       </c>
       <c r="J31" s="2" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="K31" s="2" t="n">
-        <v>563</v>
+        <v>0</v>
       </c>
       <c r="L31" s="3" t="n">
-        <v>4.058</v>
+        <v>4.86</v>
       </c>
       <c r="M31" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N31" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O31" s="2" t="n">
         <v>3</v>
@@ -2019,46 +1998,46 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>10</v>
+        <v>351</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>2</v>
+        <v>86.8</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L32" s="3" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="M32" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="J32" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K32" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" s="3" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="M32" s="4" t="n">
-        <v>10</v>
-      </c>
       <c r="N32" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O32" s="2" t="n">
         <v>3</v>
@@ -2066,46 +2045,46 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>1.2</v>
+        <v>1.9</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="G33" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>201.4</v>
+        <v>5.6</v>
       </c>
       <c r="J33" s="2" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="K33" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33" s="3" t="n">
-        <v>2.6</v>
+        <v>3.3</v>
       </c>
       <c r="M33" s="4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N33" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O33" s="2" t="n">
         <v>3</v>
@@ -2113,46 +2092,46 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>4.9</v>
+        <v>2.7</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>1.1</v>
+        <v>1.4</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>100.2</v>
+        <v>9.6</v>
       </c>
       <c r="J34" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K34" s="2" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L34" s="3" t="n">
-        <v>1.5</v>
+        <v>3.12</v>
       </c>
       <c r="M34" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N34" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O34" s="2" t="n">
         <v>3</v>
@@ -2160,46 +2139,46 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>5.5</v>
+        <v>3.9</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F35" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>158.2</v>
+        <v>18.7</v>
       </c>
       <c r="J35" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="K35" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L35" s="3" t="n">
-        <v>4.86</v>
+        <v>1.9</v>
       </c>
       <c r="M35" s="4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N35" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O35" s="2" t="n">
         <v>3</v>
@@ -2207,46 +2186,46 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>351</v>
+        <v>31</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>86.8</v>
+        <v>7.2</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>0.4</v>
+        <v>1.9</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="I36" s="2" t="n">
-        <v>0</v>
+        <v>43.2</v>
       </c>
       <c r="J36" s="2" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K36" s="2" t="n">
         <v>2</v>
       </c>
       <c r="L36" s="3" t="n">
-        <v>3.21</v>
+        <v>2.79</v>
       </c>
       <c r="M36" s="4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N36" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O36" s="2" t="n">
         <v>3</v>
@@ -2254,46 +2233,46 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>6.4</v>
+        <v>2.2</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="I37" s="2" t="n">
-        <v>5.6</v>
+        <v>46.3</v>
       </c>
       <c r="J37" s="2" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="K37" s="2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L37" s="3" t="n">
-        <v>3.3</v>
+        <v>5.99</v>
       </c>
       <c r="M37" s="4" t="n">
         <v>10</v>
       </c>
       <c r="N37" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O37" s="2" t="n">
         <v>3</v>
@@ -2301,46 +2280,46 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>2.7</v>
+        <v>5.7</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>0.4</v>
+        <v>3.2</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="I38" s="2" t="n">
-        <v>9.6</v>
+        <v>51.7</v>
       </c>
       <c r="J38" s="2" t="n">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="K38" s="2" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="L38" s="3" t="n">
-        <v>3.12</v>
+        <v>8.63</v>
       </c>
       <c r="M38" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N38" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O38" s="2" t="n">
         <v>3</v>
@@ -2348,46 +2327,46 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>3.9</v>
+        <v>5.4</v>
       </c>
       <c r="E39" s="2" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="F39" s="2" t="n">
         <v>0.9</v>
       </c>
-      <c r="F39" s="2" t="n">
-        <v>0.1</v>
-      </c>
       <c r="G39" s="2" t="n">
-        <v>0.2</v>
+        <v>1.9</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>18.7</v>
+        <v>17.9</v>
       </c>
       <c r="J39" s="2" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="K39" s="2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L39" s="3" t="n">
-        <v>1.9</v>
+        <v>2.2</v>
       </c>
       <c r="M39" s="4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N39" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O39" s="2" t="n">
         <v>3</v>
@@ -2395,46 +2374,46 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>7.2</v>
+        <v>3.1</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>1.9</v>
+        <v>1.1</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>43.2</v>
+        <v>21.2</v>
       </c>
       <c r="J40" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="K40" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L40" s="3" t="n">
-        <v>2.79</v>
+        <v>1.08</v>
       </c>
       <c r="M40" s="4" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N40" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O40" s="2" t="n">
         <v>3</v>
@@ -2442,46 +2421,46 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>2.2</v>
+        <v>5.3</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>1.8</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="H41" s="2" t="n">
         <v>18</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>46.3</v>
+        <v>1.2</v>
       </c>
       <c r="J41" s="2" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="K41" s="2" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L41" s="3" t="n">
-        <v>5.99</v>
+        <v>2.99</v>
       </c>
       <c r="M41" s="4" t="n">
         <v>10</v>
       </c>
       <c r="N41" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O41" s="2" t="n">
         <v>3</v>
@@ -2489,40 +2468,40 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>5.7</v>
+        <v>19.3</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>3.3</v>
+        <v>0.4</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>3.2</v>
+        <v>0.1</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>51.7</v>
+        <v>29.6</v>
       </c>
       <c r="J42" s="2" t="n">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="K42" s="2" t="n">
         <v>2</v>
       </c>
       <c r="L42" s="3" t="n">
-        <v>8.63</v>
+        <v>2.9</v>
       </c>
       <c r="M42" s="4" t="n">
         <v>5</v>
@@ -2531,189 +2510,189 @@
         <v>7</v>
       </c>
       <c r="O42" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
-        <v>156</v>
+        <v>190</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>5.4</v>
+        <v>11.5</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>2.9</v>
+        <v>0.9</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>1.9</v>
+        <v>0.2</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="I43" s="2" t="n">
-        <v>17.9</v>
+        <v>60.9</v>
       </c>
       <c r="J43" s="2" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="K43" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L43" s="3" t="n">
-        <v>2.2</v>
+        <v>1.66</v>
       </c>
       <c r="M43" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N43" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O43" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>3.1</v>
+        <v>18.9</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>1.1</v>
+        <v>1.4</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I44" s="2" t="n">
-        <v>21.2</v>
+        <v>27</v>
       </c>
       <c r="J44" s="2" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K44" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L44" s="3" t="n">
-        <v>1.08</v>
+        <v>4.98</v>
       </c>
       <c r="M44" s="4" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="N44" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O44" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
-        <v>162</v>
+        <v>192</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>5.3</v>
+        <v>10.4</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H45" s="2" t="n">
         <v>18</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>1.2</v>
+        <v>24.5</v>
       </c>
       <c r="J45" s="2" t="n">
         <v>0.3</v>
       </c>
       <c r="K45" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L45" s="3" t="n">
-        <v>2.99</v>
+        <v>1.5</v>
       </c>
       <c r="M45" s="4" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N45" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O45" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>19.3</v>
+        <v>13</v>
       </c>
       <c r="E46" s="2" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="F46" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="F46" s="2" t="n">
-        <v>0.1</v>
-      </c>
       <c r="G46" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>29.6</v>
+        <v>80.6</v>
       </c>
       <c r="J46" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K46" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L46" s="3" t="n">
-        <v>2.9</v>
+        <v>1.59</v>
       </c>
       <c r="M46" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N46" s="4" t="n">
         <v>7</v>
@@ -2724,19 +2703,19 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>11.5</v>
+        <v>15.8</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="F47" s="2" t="n">
         <v>0.2</v>
@@ -2745,19 +2724,19 @@
         <v>0.2</v>
       </c>
       <c r="H47" s="2" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I47" s="2" t="n">
-        <v>60.9</v>
+        <v>19.1</v>
       </c>
       <c r="J47" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K47" s="2" t="n">
         <v>4</v>
       </c>
       <c r="L47" s="3" t="n">
-        <v>1.66</v>
+        <v>2.29</v>
       </c>
       <c r="M47" s="4" t="n">
         <v>5</v>
@@ -2771,40 +2750,40 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>18.9</v>
+        <v>15.3</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>1.4</v>
+        <v>0.6</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H48" s="2" t="n">
         <v>18</v>
       </c>
       <c r="I48" s="2" t="n">
-        <v>27</v>
+        <v>16.2</v>
       </c>
       <c r="J48" s="2" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="K48" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L48" s="3" t="n">
-        <v>4.98</v>
+        <v>3.99</v>
       </c>
       <c r="M48" s="4" t="n">
         <v>5</v>
@@ -2818,43 +2797,43 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>10.4</v>
+        <v>22.5</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="I49" s="2" t="n">
-        <v>24.5</v>
+        <v>14.8</v>
       </c>
       <c r="J49" s="2" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K49" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L49" s="3" t="n">
-        <v>1.5</v>
+        <v>2.1</v>
       </c>
       <c r="M49" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N49" s="4" t="n">
         <v>7</v>
@@ -2865,43 +2844,43 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>13</v>
+        <v>6.5</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>1.1</v>
+        <v>0.9</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I50" s="2" t="n">
-        <v>80.6</v>
+        <v>3.8</v>
       </c>
       <c r="J50" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K50" s="2" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="L50" s="3" t="n">
-        <v>1.59</v>
+        <v>8.5</v>
       </c>
       <c r="M50" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N50" s="4" t="n">
         <v>7</v>
@@ -2912,40 +2891,40 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>15.8</v>
+        <v>11.5</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>0.8</v>
+        <v>1.3</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H51" s="2" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="I51" s="2" t="n">
-        <v>19.1</v>
+        <v>70.8</v>
       </c>
       <c r="J51" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K51" s="2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L51" s="3" t="n">
-        <v>2.29</v>
+        <v>1.7</v>
       </c>
       <c r="M51" s="4" t="n">
         <v>5</v>
@@ -2959,19 +2938,19 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>15.3</v>
+        <v>11.5</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>0.6</v>
+        <v>1.1</v>
       </c>
       <c r="F52" s="2" t="n">
         <v>0.1</v>
@@ -2980,22 +2959,22 @@
         <v>0.1</v>
       </c>
       <c r="H52" s="2" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I52" s="2" t="n">
-        <v>16.2</v>
+        <v>43.5</v>
       </c>
       <c r="J52" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="K52" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52" s="3" t="n">
-        <v>3.99</v>
+        <v>1.69</v>
       </c>
       <c r="M52" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N52" s="4" t="n">
         <v>7</v>
@@ -3006,40 +2985,40 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>22.5</v>
+        <v>11.1</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="I53" s="2" t="n">
-        <v>14.8</v>
+        <v>38.2</v>
       </c>
       <c r="J53" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="K53" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L53" s="3" t="n">
-        <v>2.1</v>
+        <v>0.298</v>
       </c>
       <c r="M53" s="4" t="n">
         <v>5</v>
@@ -3053,43 +3032,43 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>6.5</v>
+        <v>16.6</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G54" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="H54" s="2" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="J54" s="2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K54" s="2" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="L54" s="3" t="n">
-        <v>8.5</v>
+        <v>1.99</v>
       </c>
       <c r="M54" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N54" s="4" t="n">
         <v>7</v>
@@ -3100,43 +3079,43 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>11.5</v>
+        <v>10.4</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>1.3</v>
+        <v>0.5</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H55" s="2" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I55" s="2" t="n">
-        <v>70.8</v>
+        <v>82.2</v>
       </c>
       <c r="J55" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K55" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L55" s="3" t="n">
-        <v>1.7</v>
+        <v>1.19</v>
       </c>
       <c r="M55" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N55" s="4" t="n">
         <v>7</v>
@@ -3147,40 +3126,40 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>11.5</v>
+        <v>19.4</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>1.1</v>
+        <v>0.4</v>
       </c>
       <c r="F56" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G56" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="H56" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I56" s="2" t="n">
-        <v>43.5</v>
+        <v>65.5</v>
       </c>
       <c r="J56" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K56" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L56" s="3" t="n">
-        <v>1.69</v>
+        <v>0.99</v>
       </c>
       <c r="M56" s="4" t="n">
         <v>8</v>
@@ -3194,40 +3173,40 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>11.1</v>
+        <v>12.3</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="F57" s="2" t="n">
-        <v>0.1</v>
+        <v>2.1</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="H57" s="2" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I57" s="2" t="n">
-        <v>38.2</v>
+        <v>19.8</v>
       </c>
       <c r="J57" s="2" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="K57" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L57" s="3" t="n">
-        <v>0.298</v>
+        <v>2.268</v>
       </c>
       <c r="M57" s="4" t="n">
         <v>5</v>
@@ -3241,40 +3220,40 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="D58" s="2" t="n">
-        <v>16.6</v>
+        <v>8.1</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="F58" s="2" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G58" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H58" s="2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I58" s="2" t="n">
-        <v>1.5</v>
+        <v>6.1</v>
       </c>
       <c r="J58" s="2" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K58" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L58" s="3" t="n">
-        <v>1.99</v>
+        <v>0.299</v>
       </c>
       <c r="M58" s="4" t="n">
         <v>8</v>
@@ -3288,40 +3267,40 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D59" s="2" t="n">
-        <v>10.4</v>
+        <v>7.5</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F59" s="2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G59" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="H59" s="2" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I59" s="2" t="n">
-        <v>82.2</v>
+        <v>8.7</v>
       </c>
       <c r="J59" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K59" s="2" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="L59" s="3" t="n">
-        <v>1.19</v>
+        <v>0.6</v>
       </c>
       <c r="M59" s="4" t="n">
         <v>8</v>
@@ -3335,37 +3314,37 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D60" s="2" t="n">
-        <v>19.4</v>
+        <v>14.9</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="F60" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G60" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="H60" s="2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I60" s="2" t="n">
-        <v>65.5</v>
+        <v>21.8</v>
       </c>
       <c r="J60" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K60" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L60" s="3" t="n">
         <v>0.99</v>
@@ -3382,43 +3361,43 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="D61" s="2" t="n">
-        <v>12.3</v>
+        <v>6.8</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="F61" s="2" t="n">
-        <v>2.1</v>
+        <v>0.3</v>
       </c>
       <c r="G61" s="2" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="H61" s="2" t="n">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I61" s="2" t="n">
-        <v>19.8</v>
+        <v>63.6</v>
       </c>
       <c r="J61" s="2" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="K61" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L61" s="3" t="n">
-        <v>2.268</v>
+        <v>5.2</v>
       </c>
       <c r="M61" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N61" s="4" t="n">
         <v>7</v>
@@ -3429,43 +3408,43 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>33</v>
+        <v>205</v>
       </c>
       <c r="D62" s="2" t="n">
-        <v>8.1</v>
+        <v>13</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>0.9</v>
+        <v>2.3</v>
       </c>
       <c r="F62" s="2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G62" s="2" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H62" s="2" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I62" s="2" t="n">
-        <v>6.1</v>
+        <v>8.3</v>
       </c>
       <c r="J62" s="2" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="K62" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L62" s="3" t="n">
-        <v>0.299</v>
+        <v>15.9</v>
       </c>
       <c r="M62" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N62" s="4" t="n">
         <v>7</v>
@@ -3476,40 +3455,40 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D63" s="2" t="n">
-        <v>7.5</v>
+        <v>14</v>
       </c>
       <c r="E63" s="2" t="n">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="F63" s="2" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G63" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H63" s="2" t="n">
         <v>6</v>
       </c>
       <c r="I63" s="2" t="n">
-        <v>8.7</v>
+        <v>2.8</v>
       </c>
       <c r="J63" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K63" s="2" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L63" s="3" t="n">
-        <v>0.6</v>
+        <v>1.49</v>
       </c>
       <c r="M63" s="4" t="n">
         <v>8</v>
@@ -3523,40 +3502,40 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D64" s="2" t="n">
-        <v>14.9</v>
+        <v>9.3</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="F64" s="2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H64" s="2" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I64" s="2" t="n">
-        <v>21.8</v>
+        <v>3.3</v>
       </c>
       <c r="J64" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K64" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L64" s="3" t="n">
-        <v>0.99</v>
+        <v>3.1</v>
       </c>
       <c r="M64" s="4" t="n">
         <v>8</v>
@@ -3570,40 +3549,40 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D65" s="2" t="n">
-        <v>6.8</v>
+        <v>9.6</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="F65" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="G65" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H65" s="2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I65" s="2" t="n">
-        <v>63.6</v>
+        <v>48.8</v>
       </c>
       <c r="J65" s="2" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K65" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L65" s="3" t="n">
-        <v>5.2</v>
+        <v>0.99</v>
       </c>
       <c r="M65" s="4" t="n">
         <v>8</v>
@@ -3617,43 +3596,43 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>205</v>
+        <v>53</v>
       </c>
       <c r="D66" s="2" t="n">
-        <v>13</v>
+        <v>13.6</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>2.3</v>
+        <v>0.7</v>
       </c>
       <c r="F66" s="2" t="n">
-        <v>18</v>
+        <v>0.2</v>
       </c>
       <c r="G66" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H66" s="2" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="I66" s="2" t="n">
-        <v>8.3</v>
+        <v>3.3</v>
       </c>
       <c r="J66" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K66" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L66" s="3" t="n">
-        <v>15.9</v>
+        <v>2</v>
       </c>
       <c r="M66" s="4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N66" s="4" t="n">
         <v>7</v>
@@ -3664,43 +3643,43 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
-        <v>243</v>
+        <v>175</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D67" s="2" t="n">
-        <v>14</v>
+        <v>33.7</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>0.6</v>
+        <v>1.4</v>
       </c>
       <c r="F67" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G67" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H67" s="2" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="I67" s="2" t="n">
-        <v>2.8</v>
+        <v>15.7</v>
       </c>
       <c r="J67" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K67" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L67" s="3" t="n">
-        <v>1.49</v>
+        <v>1.65</v>
       </c>
       <c r="M67" s="4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N67" s="4" t="n">
         <v>7</v>
@@ -3711,894 +3690,565 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
-        <v>244</v>
+        <v>491</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>36</v>
+        <v>401</v>
       </c>
       <c r="D68" s="2" t="n">
-        <v>9.3</v>
+        <v>91.2</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>0.8</v>
+        <v>4.2</v>
       </c>
       <c r="F68" s="2" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="G68" s="2" t="n">
-        <v>0.2</v>
+        <v>5.4</v>
       </c>
       <c r="H68" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="I68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K68" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="L68" s="3" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="M68" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="I68" s="2" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="J68" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K68" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L68" s="3" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="M68" s="4" t="n">
-        <v>8</v>
-      </c>
       <c r="N68" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O68" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
-        <v>251</v>
+        <v>495</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>38</v>
+        <v>540</v>
       </c>
       <c r="D69" s="2" t="n">
-        <v>9.6</v>
+        <v>59.6</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>0.8</v>
+        <v>7.2</v>
       </c>
       <c r="F69" s="2" t="n">
-        <v>0.1</v>
+        <v>30.3</v>
       </c>
       <c r="G69" s="2" t="n">
-        <v>0.1</v>
+        <v>1.6</v>
       </c>
       <c r="H69" s="2" t="n">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="I69" s="2" t="n">
-        <v>48.8</v>
+        <v>0</v>
       </c>
       <c r="J69" s="2" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="K69" s="2" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="L69" s="3" t="n">
-        <v>0.99</v>
+        <v>5.99</v>
       </c>
       <c r="M69" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N69" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O69" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
-        <v>256</v>
+        <v>498</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>53</v>
+        <v>475</v>
       </c>
       <c r="D70" s="2" t="n">
-        <v>13.6</v>
+        <v>62.4</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>0.7</v>
+        <v>4.9</v>
       </c>
       <c r="F70" s="2" t="n">
-        <v>0.2</v>
+        <v>29.9</v>
       </c>
       <c r="G70" s="2" t="n">
-        <v>0.1</v>
+        <v>3.6</v>
       </c>
       <c r="H70" s="2" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="I70" s="2" t="n">
-        <v>3.3</v>
+        <v>2.1</v>
       </c>
       <c r="J70" s="2" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K70" s="2" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L70" s="3" t="n">
-        <v>2</v>
+        <v>11.29</v>
       </c>
       <c r="M70" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N70" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O70" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
-        <v>175</v>
+        <v>499</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>128</v>
+        <v>449</v>
       </c>
       <c r="D71" s="2" t="n">
-        <v>33.7</v>
+        <v>81.4</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>1.4</v>
+        <v>1.1</v>
       </c>
       <c r="F71" s="2" t="n">
-        <v>0.2</v>
+        <v>13.6</v>
       </c>
       <c r="G71" s="2" t="n">
-        <v>0.3</v>
+        <v>1.2</v>
       </c>
       <c r="H71" s="2" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I71" s="2" t="n">
-        <v>15.7</v>
+        <v>0</v>
       </c>
       <c r="J71" s="2" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="K71" s="2" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="L71" s="3" t="n">
-        <v>1.65</v>
+        <v>8.39</v>
       </c>
       <c r="M71" s="4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N71" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O71" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
-        <v>491</v>
+        <v>561</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>401</v>
+        <v>76</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>91.2</v>
+        <v>13.6</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>4.2</v>
+        <v>4.8</v>
       </c>
       <c r="F72" s="2" t="n">
-        <v>2.2</v>
+        <v>0.5</v>
       </c>
       <c r="G72" s="2" t="n">
-        <v>5.4</v>
+        <v>1.3</v>
       </c>
       <c r="H72" s="2" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="I72" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J72" s="2" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="K72" s="2" t="n">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="L72" s="3" t="n">
-        <v>2.67</v>
+        <v>0.699</v>
       </c>
       <c r="M72" s="4" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="N72" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O72" s="2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
-        <v>492</v>
+        <v>558</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>387</v>
+        <v>606</v>
       </c>
       <c r="D73" s="2" t="n">
-        <v>99.6</v>
+        <v>18.7</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>0.3</v>
+        <v>22.5</v>
       </c>
       <c r="F73" s="2" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G73" s="2" t="n">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="H73" s="2" t="n">
+        <v>159</v>
+      </c>
+      <c r="I73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K73" s="2" t="n">
+        <v>376</v>
+      </c>
+      <c r="L73" s="3" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="M73" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N73" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I73" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J73" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K73" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L73" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M73" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="N73" s="4" t="n">
-        <v>7</v>
-      </c>
       <c r="O73" s="2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
-        <v>493</v>
+        <v>377</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>369</v>
+        <v>219</v>
       </c>
       <c r="D74" s="2" t="n">
-        <v>94.5</v>
+        <v>0</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>0.8</v>
+        <v>35.9</v>
       </c>
       <c r="F74" s="2" t="n">
-        <v>0.1</v>
+        <v>7.3</v>
       </c>
       <c r="G74" s="2" t="n">
-        <v>8.3</v>
+        <v>3</v>
       </c>
       <c r="H74" s="2" t="n">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="I74" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J74" s="2" t="n">
-        <v>0.5</v>
+        <v>8.1</v>
       </c>
       <c r="K74" s="2" t="n">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="L74" s="3" t="n">
-        <v>2.179</v>
+        <v>5.69</v>
       </c>
       <c r="M74" s="4" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="N74" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O74" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>387</v>
+        <v>146</v>
       </c>
       <c r="D75" s="2" t="n">
-        <v>99.5</v>
+        <v>0.6</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>0.3</v>
+        <v>13.3</v>
       </c>
       <c r="F75" s="2" t="n">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="G75" s="2" t="n">
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
       <c r="H75" s="2" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I75" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J75" s="2" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="K75" s="2" t="n">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="L75" s="3" t="n">
-        <v>0.49</v>
+        <v>1.8</v>
       </c>
       <c r="M75" s="4" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="N75" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O75" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
-        <v>495</v>
+        <v>406</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>540</v>
+        <v>212</v>
       </c>
       <c r="D76" s="2" t="n">
-        <v>59.6</v>
+        <v>0</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>7.2</v>
+        <v>33.4</v>
       </c>
       <c r="F76" s="2" t="n">
-        <v>30.3</v>
+        <v>7.6</v>
       </c>
       <c r="G76" s="2" t="n">
-        <v>1.6</v>
+        <v>0.5</v>
       </c>
       <c r="H76" s="2" t="n">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="I76" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J76" s="2" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="K76" s="2" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="L76" s="3" t="n">
-        <v>5.99</v>
+        <v>2.49</v>
       </c>
       <c r="M76" s="4" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="N76" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O76" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
-        <v>498</v>
+        <v>277</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>475</v>
+        <v>166</v>
       </c>
       <c r="D77" s="2" t="n">
-        <v>62.4</v>
+        <v>0</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>4.9</v>
+        <v>26.2</v>
       </c>
       <c r="F77" s="2" t="n">
-        <v>29.9</v>
+        <v>6</v>
       </c>
       <c r="G77" s="2" t="n">
-        <v>3.6</v>
+        <v>1.2</v>
       </c>
       <c r="H77" s="2" t="n">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="I77" s="2" t="n">
-        <v>2.1</v>
+        <v>0</v>
       </c>
       <c r="J77" s="2" t="n">
-        <v>1.5</v>
+        <v>0.6</v>
       </c>
       <c r="K77" s="2" t="n">
-        <v>9</v>
+        <v>362</v>
       </c>
       <c r="L77" s="3" t="n">
-        <v>11.29</v>
+        <v>5.35</v>
       </c>
       <c r="M77" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N77" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O77" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>884</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L78" s="1" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="M78" s="1" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="n">
-        <v>499</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C78" s="2" t="n">
-        <v>449</v>
-      </c>
-      <c r="D78" s="2" t="n">
-        <v>81.4</v>
-      </c>
-      <c r="E78" s="2" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="F78" s="2" t="n">
-        <v>13.6</v>
-      </c>
-      <c r="G78" s="2" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="H78" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="I78" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J78" s="2" t="n">
+      <c r="N78" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O78" s="1" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>726</v>
+      </c>
+      <c r="D79" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E79" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="K78" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="L78" s="3" t="n">
-        <v>8.39</v>
-      </c>
-      <c r="M78" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="N78" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O78" s="2" t="n">
+      <c r="F79" s="1" t="n">
+        <v>82.4</v>
+      </c>
+      <c r="G79" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H79" s="1" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="n">
-        <v>561</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C79" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="D79" s="2" t="n">
-        <v>13.6</v>
-      </c>
-      <c r="E79" s="2" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="F79" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G79" s="2" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="H79" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="I79" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" s="2" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="K79" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="L79" s="3" t="n">
-        <v>0.699</v>
-      </c>
-      <c r="M79" s="4" t="n">
-        <v>20</v>
+      <c r="I79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" s="1" t="n">
+        <v>579</v>
+      </c>
+      <c r="L79" s="1" t="n">
+        <v>6.49</v>
+      </c>
+      <c r="M79" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="N79" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="O79" s="2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2" t="n">
-        <v>558</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C80" s="2" t="n">
-        <v>606</v>
-      </c>
-      <c r="D80" s="2" t="n">
-        <v>18.7</v>
-      </c>
-      <c r="E80" s="2" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="F80" s="2" t="n">
-        <v>54</v>
-      </c>
-      <c r="G80" s="2" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="H80" s="2" t="n">
-        <v>159</v>
-      </c>
-      <c r="I80" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J80" s="2" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="K80" s="2" t="n">
-        <v>376</v>
-      </c>
-      <c r="L80" s="3" t="n">
-        <v>3.89</v>
-      </c>
-      <c r="M80" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="N80" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O80" s="2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="n">
-        <v>377</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C81" s="2" t="n">
-        <v>219</v>
-      </c>
-      <c r="D81" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E81" s="2" t="n">
-        <v>35.9</v>
-      </c>
-      <c r="F81" s="2" t="n">
-        <v>7.3</v>
-      </c>
-      <c r="G81" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="H81" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="I81" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J81" s="2" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="K81" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="L81" s="3" t="n">
-        <v>5.69</v>
-      </c>
-      <c r="M81" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="N81" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O81" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="n">
-        <v>488</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C82" s="2" t="n">
-        <v>146</v>
-      </c>
-      <c r="D82" s="2" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="E82" s="2" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F82" s="2" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="G82" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="H82" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="I82" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J82" s="2" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="K82" s="2" t="n">
-        <v>146</v>
-      </c>
-      <c r="L82" s="3" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="M82" s="4" t="n">
-        <v>15</v>
-      </c>
-      <c r="N82" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O82" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="n">
-        <v>406</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C83" s="2" t="n">
-        <v>212</v>
-      </c>
-      <c r="D83" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E83" s="2" t="n">
-        <v>33.4</v>
-      </c>
-      <c r="F83" s="2" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="G83" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H83" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="I83" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J83" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K83" s="2" t="n">
-        <v>56</v>
-      </c>
-      <c r="L83" s="3" t="n">
-        <v>2.49</v>
-      </c>
-      <c r="M83" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="N83" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O83" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="n">
-        <v>277</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C84" s="2" t="n">
-        <v>166</v>
-      </c>
-      <c r="D84" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E84" s="2" t="n">
-        <v>26.2</v>
-      </c>
-      <c r="F84" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="G84" s="2" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="H84" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="I84" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J84" s="2" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="K84" s="2" t="n">
-        <v>362</v>
-      </c>
-      <c r="L84" s="3" t="n">
-        <v>5.35</v>
-      </c>
-      <c r="M84" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="N84" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O84" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
-        <v>260</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C85" s="0" t="n">
-        <v>884</v>
-      </c>
-      <c r="D85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F85" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L85" s="1" t="n">
-        <v>11.19</v>
-      </c>
-      <c r="M85" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N85" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O85" s="0" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
-        <v>261</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C86" s="0" t="n">
-        <v>726</v>
-      </c>
-      <c r="D86" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E86" s="0" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="F86" s="0" t="n">
-        <v>82.4</v>
-      </c>
-      <c r="G86" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H86" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I86" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J86" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K86" s="0" t="n">
-        <v>579</v>
-      </c>
-      <c r="L86" s="1" t="n">
-        <v>6.49</v>
-      </c>
-      <c r="M86" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N86" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O86" s="0" t="n">
+      <c r="O79" s="1" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correção restriçoes, mudança no tempo de execução
</commit_message>
<xml_diff>
--- a/alimentosCompleto.xlsx
+++ b/alimentosCompleto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t xml:space="preserve">pimentaoVermelho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">polvilho</t>
   </si>
   <si>
     <t xml:space="preserve">quiabo</t>
@@ -523,12 +520,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O79"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="R49" activeCellId="0" sqref="R49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1188,7 +1185,7 @@
         <v>3.75</v>
       </c>
       <c r="M14" s="4" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N14" s="4" t="n">
         <v>7</v>
@@ -1235,7 +1232,7 @@
         <v>4.5</v>
       </c>
       <c r="M15" s="4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N15" s="4" t="n">
         <v>7</v>
@@ -1282,10 +1279,10 @@
         <v>2.39</v>
       </c>
       <c r="M16" s="4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="N16" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O16" s="2" t="n">
         <v>3</v>
@@ -1423,7 +1420,7 @@
         <v>2.75</v>
       </c>
       <c r="M19" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N19" s="4" t="n">
         <v>3</v>
@@ -1470,7 +1467,7 @@
         <v>1.12</v>
       </c>
       <c r="M20" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N20" s="4" t="n">
         <v>3</v>
@@ -1517,7 +1514,7 @@
         <v>0.5</v>
       </c>
       <c r="M21" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N21" s="4" t="n">
         <v>3</v>
@@ -1564,7 +1561,7 @@
         <v>1.39</v>
       </c>
       <c r="M22" s="4" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="N22" s="4" t="n">
         <v>3</v>
@@ -1661,7 +1658,7 @@
         <v>12</v>
       </c>
       <c r="N24" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O24" s="2" t="n">
         <v>3</v>
@@ -1752,7 +1749,7 @@
         <v>1.92</v>
       </c>
       <c r="M26" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N26" s="4" t="n">
         <v>3</v>
@@ -1802,7 +1799,7 @@
         <v>8</v>
       </c>
       <c r="N27" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O27" s="2" t="n">
         <v>3</v>
@@ -1846,10 +1843,10 @@
         <v>0.95</v>
       </c>
       <c r="M28" s="4" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N28" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O28" s="2" t="n">
         <v>3</v>
@@ -1893,10 +1890,10 @@
         <v>2.6</v>
       </c>
       <c r="M29" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N29" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O29" s="2" t="n">
         <v>3</v>
@@ -1940,10 +1937,10 @@
         <v>1.5</v>
       </c>
       <c r="M30" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N30" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O30" s="2" t="n">
         <v>3</v>
@@ -1987,10 +1984,10 @@
         <v>4.86</v>
       </c>
       <c r="M31" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N31" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O31" s="2" t="n">
         <v>3</v>
@@ -1998,43 +1995,43 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>351</v>
+        <v>30</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>86.8</v>
+        <v>6.4</v>
       </c>
       <c r="E32" s="2" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G32" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="F32" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2" t="n">
-        <v>0.5</v>
-      </c>
       <c r="H32" s="2" t="n">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="J32" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="K32" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L32" s="3" t="n">
-        <v>3.21</v>
+        <v>3.3</v>
       </c>
       <c r="M32" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N32" s="4" t="n">
         <v>3</v>
@@ -2045,43 +2042,43 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>6.4</v>
+        <v>2.7</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="G33" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>5.6</v>
+        <v>9.6</v>
       </c>
       <c r="J33" s="2" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="K33" s="2" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L33" s="3" t="n">
-        <v>3.3</v>
+        <v>3.12</v>
       </c>
       <c r="M33" s="4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N33" s="4" t="n">
         <v>3</v>
@@ -2092,43 +2089,43 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>2.7</v>
+        <v>3.9</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>9.6</v>
+        <v>18.7</v>
       </c>
       <c r="J34" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="K34" s="2" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="L34" s="3" t="n">
-        <v>3.12</v>
+        <v>1.9</v>
       </c>
       <c r="M34" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N34" s="4" t="n">
         <v>3</v>
@@ -2139,43 +2136,43 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>3.9</v>
+        <v>7.2</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>0.9</v>
+        <v>1.9</v>
       </c>
       <c r="F35" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>18.7</v>
+        <v>43.2</v>
       </c>
       <c r="J35" s="2" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="K35" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L35" s="3" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="M35" s="4" t="n">
         <v>4</v>
-      </c>
-      <c r="L35" s="3" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="M35" s="4" t="n">
-        <v>10</v>
       </c>
       <c r="N35" s="4" t="n">
         <v>3</v>
@@ -2186,46 +2183,46 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>7.2</v>
+        <v>2.2</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="F36" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="H36" s="2" t="n">
         <v>18</v>
       </c>
       <c r="I36" s="2" t="n">
-        <v>43.2</v>
+        <v>46.3</v>
       </c>
       <c r="J36" s="2" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K36" s="2" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L36" s="3" t="n">
-        <v>2.79</v>
+        <v>5.99</v>
       </c>
       <c r="M36" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N36" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O36" s="2" t="n">
         <v>3</v>
@@ -2233,43 +2230,43 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>2.2</v>
+        <v>5.7</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>1.8</v>
+        <v>3.3</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>0.9</v>
+        <v>3.2</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I37" s="2" t="n">
-        <v>46.3</v>
+        <v>51.7</v>
       </c>
       <c r="J37" s="2" t="n">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="K37" s="2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L37" s="3" t="n">
-        <v>5.99</v>
+        <v>8.63</v>
       </c>
       <c r="M37" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N37" s="4" t="n">
         <v>3</v>
@@ -2280,43 +2277,43 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>5.7</v>
+        <v>5.4</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>3.3</v>
+        <v>2.9</v>
       </c>
       <c r="F38" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="J38" s="2" t="n">
         <v>0.6</v>
       </c>
-      <c r="G38" s="2" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="H38" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="I38" s="2" t="n">
-        <v>51.7</v>
-      </c>
-      <c r="J38" s="2" t="n">
-        <v>1.3</v>
-      </c>
       <c r="K38" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L38" s="3" t="n">
-        <v>8.63</v>
+        <v>2.2</v>
       </c>
       <c r="M38" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N38" s="4" t="n">
         <v>3</v>
@@ -2327,43 +2324,43 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>5.4</v>
+        <v>3.1</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>2.9</v>
+        <v>1.1</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>1.9</v>
+        <v>0.2</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>17.9</v>
+        <v>21.2</v>
       </c>
       <c r="J39" s="2" t="n">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="K39" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L39" s="3" t="n">
-        <v>2.2</v>
+        <v>1.08</v>
       </c>
       <c r="M39" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N39" s="4" t="n">
         <v>3</v>
@@ -2374,43 +2371,43 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>3.1</v>
+        <v>5.3</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>1.1</v>
+        <v>1.8</v>
       </c>
       <c r="F40" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>21.2</v>
+        <v>1.2</v>
       </c>
       <c r="J40" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="K40" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="3" t="n">
-        <v>1.08</v>
+        <v>2.99</v>
       </c>
       <c r="M40" s="4" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="N40" s="4" t="n">
         <v>3</v>
@@ -2421,93 +2418,93 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>5.3</v>
+        <v>19.3</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>1.8</v>
+        <v>0.4</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>1.2</v>
+        <v>29.6</v>
       </c>
       <c r="J41" s="2" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K41" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L41" s="3" t="n">
-        <v>2.99</v>
+        <v>2.9</v>
       </c>
       <c r="M41" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N41" s="4" t="n">
         <v>3</v>
       </c>
       <c r="O41" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>19.3</v>
+        <v>11.5</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>29.6</v>
+        <v>60.9</v>
       </c>
       <c r="J42" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="K42" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L42" s="3" t="n">
-        <v>2.9</v>
+        <v>1.66</v>
       </c>
       <c r="M42" s="4" t="n">
         <v>5</v>
       </c>
       <c r="N42" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O42" s="2" t="n">
         <v>2</v>
@@ -2515,46 +2512,46 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>11.5</v>
+        <v>18.9</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I43" s="2" t="n">
-        <v>60.9</v>
+        <v>27</v>
       </c>
       <c r="J43" s="2" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K43" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L43" s="3" t="n">
-        <v>1.66</v>
+        <v>4.98</v>
       </c>
       <c r="M43" s="4" t="n">
         <v>5</v>
       </c>
       <c r="N43" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O43" s="2" t="n">
         <v>2</v>
@@ -2562,46 +2559,46 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>18.9</v>
+        <v>10.4</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H44" s="2" t="n">
         <v>18</v>
       </c>
       <c r="I44" s="2" t="n">
-        <v>27</v>
+        <v>24.5</v>
       </c>
       <c r="J44" s="2" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="K44" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L44" s="3" t="n">
-        <v>4.98</v>
+        <v>1.5</v>
       </c>
       <c r="M44" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N44" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O44" s="2" t="n">
         <v>2</v>
@@ -2609,46 +2606,46 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>10.4</v>
+        <v>13</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="H45" s="2" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>24.5</v>
+        <v>80.6</v>
       </c>
       <c r="J45" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="K45" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L45" s="3" t="n">
-        <v>1.5</v>
+        <v>1.59</v>
       </c>
       <c r="M45" s="4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N45" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O45" s="2" t="n">
         <v>2</v>
@@ -2656,46 +2653,46 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>13</v>
+        <v>15.8</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>1.1</v>
+        <v>0.8</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>80.6</v>
+        <v>19.1</v>
       </c>
       <c r="J46" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K46" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L46" s="3" t="n">
-        <v>1.59</v>
+        <v>2.29</v>
       </c>
       <c r="M46" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N46" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O46" s="2" t="n">
         <v>2</v>
@@ -2703,46 +2700,46 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>15.8</v>
+        <v>15.3</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H47" s="2" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I47" s="2" t="n">
-        <v>19.1</v>
+        <v>16.2</v>
       </c>
       <c r="J47" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="K47" s="2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L47" s="3" t="n">
-        <v>2.29</v>
+        <v>3.99</v>
       </c>
       <c r="M47" s="4" t="n">
         <v>5</v>
       </c>
       <c r="N47" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O47" s="2" t="n">
         <v>2</v>
@@ -2750,46 +2747,46 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>15.3</v>
+        <v>22.5</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>0.6</v>
+        <v>1.4</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="H48" s="2" t="n">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="I48" s="2" t="n">
-        <v>16.2</v>
+        <v>14.8</v>
       </c>
       <c r="J48" s="2" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K48" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L48" s="3" t="n">
-        <v>3.99</v>
+        <v>2.1</v>
       </c>
       <c r="M48" s="4" t="n">
         <v>5</v>
       </c>
       <c r="N48" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O48" s="2" t="n">
         <v>2</v>
@@ -2797,46 +2794,46 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>22.5</v>
+        <v>6.5</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="I49" s="2" t="n">
-        <v>14.8</v>
+        <v>3.8</v>
       </c>
       <c r="J49" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K49" s="2" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="L49" s="3" t="n">
-        <v>2.1</v>
+        <v>8.5</v>
       </c>
       <c r="M49" s="4" t="n">
         <v>5</v>
       </c>
       <c r="N49" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O49" s="2" t="n">
         <v>2</v>
@@ -2844,46 +2841,46 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>6.5</v>
+        <v>11.5</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I50" s="2" t="n">
-        <v>3.8</v>
+        <v>70.8</v>
       </c>
       <c r="J50" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K50" s="2" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="L50" s="3" t="n">
-        <v>8.5</v>
+        <v>1.7</v>
       </c>
       <c r="M50" s="4" t="n">
         <v>5</v>
       </c>
       <c r="N50" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O50" s="2" t="n">
         <v>2</v>
@@ -2891,46 +2888,46 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D51" s="2" t="n">
         <v>11.5</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H51" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I51" s="2" t="n">
-        <v>70.8</v>
+        <v>43.5</v>
       </c>
       <c r="J51" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K51" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" s="3" t="n">
-        <v>1.7</v>
+        <v>1.69</v>
       </c>
       <c r="M51" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N51" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O51" s="2" t="n">
         <v>2</v>
@@ -2938,46 +2935,46 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>11.5</v>
+        <v>11.1</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>1.1</v>
+        <v>0.9</v>
       </c>
       <c r="F52" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H52" s="2" t="n">
         <v>10</v>
       </c>
       <c r="I52" s="2" t="n">
-        <v>43.5</v>
+        <v>38.2</v>
       </c>
       <c r="J52" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K52" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L52" s="3" t="n">
-        <v>1.69</v>
+        <v>0.298</v>
       </c>
       <c r="M52" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N52" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O52" s="2" t="n">
         <v>2</v>
@@ -2985,46 +2982,46 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>11.1</v>
+        <v>16.6</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I53" s="2" t="n">
-        <v>38.2</v>
+        <v>1.5</v>
       </c>
       <c r="J53" s="2" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K53" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L53" s="3" t="n">
-        <v>0.298</v>
+        <v>1.99</v>
       </c>
       <c r="M53" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N53" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O53" s="2" t="n">
         <v>2</v>
@@ -3032,46 +3029,46 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>16.6</v>
+        <v>10.4</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H54" s="2" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>1.5</v>
+        <v>82.2</v>
       </c>
       <c r="J54" s="2" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K54" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L54" s="3" t="n">
-        <v>1.99</v>
+        <v>1.19</v>
       </c>
       <c r="M54" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N54" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O54" s="2" t="n">
         <v>2</v>
@@ -3079,31 +3076,31 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>10.4</v>
+        <v>19.4</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H55" s="2" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="I55" s="2" t="n">
-        <v>82.2</v>
+        <v>65.5</v>
       </c>
       <c r="J55" s="2" t="n">
         <v>0.1</v>
@@ -3112,13 +3109,13 @@
         <v>2</v>
       </c>
       <c r="L55" s="3" t="n">
-        <v>1.19</v>
+        <v>0.99</v>
       </c>
       <c r="M55" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N55" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O55" s="2" t="n">
         <v>2</v>
@@ -3126,46 +3123,46 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>19.4</v>
+        <v>12.3</v>
       </c>
       <c r="E56" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="I56" s="2" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="J56" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="F56" s="2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G56" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H56" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="I56" s="2" t="n">
-        <v>65.5</v>
-      </c>
-      <c r="J56" s="2" t="n">
-        <v>0.1</v>
-      </c>
       <c r="K56" s="2" t="n">
         <v>2</v>
       </c>
       <c r="L56" s="3" t="n">
-        <v>0.99</v>
+        <v>2.268</v>
       </c>
       <c r="M56" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N56" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O56" s="2" t="n">
         <v>2</v>
@@ -3173,46 +3170,46 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>12.3</v>
+        <v>8.1</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="F57" s="2" t="n">
-        <v>2.1</v>
+        <v>0</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="H57" s="2" t="n">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I57" s="2" t="n">
-        <v>19.8</v>
+        <v>6.1</v>
       </c>
       <c r="J57" s="2" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="K57" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L57" s="3" t="n">
-        <v>2.268</v>
+        <v>0.299</v>
       </c>
       <c r="M57" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N57" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O57" s="2" t="n">
         <v>2</v>
@@ -3220,19 +3217,19 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D58" s="2" t="n">
-        <v>8.1</v>
+        <v>7.5</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="F58" s="2" t="n">
         <v>0</v>
@@ -3241,25 +3238,25 @@
         <v>0.2</v>
       </c>
       <c r="H58" s="2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I58" s="2" t="n">
-        <v>6.1</v>
+        <v>8.7</v>
       </c>
       <c r="J58" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K58" s="2" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L58" s="3" t="n">
-        <v>0.299</v>
+        <v>0.6</v>
       </c>
       <c r="M58" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N58" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O58" s="2" t="n">
         <v>2</v>
@@ -3267,46 +3264,46 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="D59" s="2" t="n">
-        <v>7.5</v>
+        <v>14.9</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="F59" s="2" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H59" s="2" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I59" s="2" t="n">
-        <v>8.7</v>
+        <v>21.8</v>
       </c>
       <c r="J59" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="K59" s="2" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="L59" s="3" t="n">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="M59" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N59" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O59" s="2" t="n">
         <v>2</v>
@@ -3314,46 +3311,46 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D60" s="2" t="n">
-        <v>14.9</v>
+        <v>6.8</v>
       </c>
       <c r="E60" s="2" t="n">
         <v>0.9</v>
       </c>
       <c r="F60" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G60" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H60" s="2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I60" s="2" t="n">
-        <v>21.8</v>
+        <v>63.6</v>
       </c>
       <c r="J60" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K60" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L60" s="3" t="n">
-        <v>0.99</v>
+        <v>5.2</v>
       </c>
       <c r="M60" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N60" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O60" s="2" t="n">
         <v>2</v>
@@ -3361,46 +3358,46 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>30</v>
+        <v>205</v>
       </c>
       <c r="D61" s="2" t="n">
-        <v>6.8</v>
+        <v>13</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>0.9</v>
+        <v>2.3</v>
       </c>
       <c r="F61" s="2" t="n">
-        <v>0.3</v>
+        <v>18</v>
       </c>
       <c r="G61" s="2" t="n">
         <v>0.3</v>
       </c>
       <c r="H61" s="2" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I61" s="2" t="n">
-        <v>63.6</v>
+        <v>8.3</v>
       </c>
       <c r="J61" s="2" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="K61" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L61" s="3" t="n">
-        <v>5.2</v>
+        <v>15.9</v>
       </c>
       <c r="M61" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N61" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O61" s="2" t="n">
         <v>2</v>
@@ -3408,46 +3405,46 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>205</v>
+        <v>53</v>
       </c>
       <c r="D62" s="2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>2.3</v>
+        <v>0.6</v>
       </c>
       <c r="F62" s="2" t="n">
-        <v>18</v>
+        <v>0.1</v>
       </c>
       <c r="G62" s="2" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H62" s="2" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="I62" s="2" t="n">
-        <v>8.3</v>
+        <v>2.8</v>
       </c>
       <c r="J62" s="2" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="K62" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L62" s="3" t="n">
-        <v>15.9</v>
+        <v>1.49</v>
       </c>
       <c r="M62" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N62" s="4" t="n">
         <v>4</v>
-      </c>
-      <c r="N62" s="4" t="n">
-        <v>7</v>
       </c>
       <c r="O62" s="2" t="n">
         <v>2</v>
@@ -3455,31 +3452,31 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D63" s="2" t="n">
-        <v>14</v>
+        <v>9.3</v>
       </c>
       <c r="E63" s="2" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="F63" s="2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G63" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H63" s="2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I63" s="2" t="n">
-        <v>2.8</v>
+        <v>3.3</v>
       </c>
       <c r="J63" s="2" t="n">
         <v>0.1</v>
@@ -3488,13 +3485,13 @@
         <v>0</v>
       </c>
       <c r="L63" s="3" t="n">
-        <v>1.49</v>
+        <v>3.1</v>
       </c>
       <c r="M63" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N63" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O63" s="2" t="n">
         <v>2</v>
@@ -3502,46 +3499,46 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D64" s="2" t="n">
-        <v>9.3</v>
+        <v>9.6</v>
       </c>
       <c r="E64" s="2" t="n">
         <v>0.8</v>
       </c>
       <c r="F64" s="2" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G64" s="2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H64" s="2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I64" s="2" t="n">
-        <v>3.3</v>
+        <v>48.8</v>
       </c>
       <c r="J64" s="2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K64" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L64" s="3" t="n">
-        <v>3.1</v>
+        <v>0.99</v>
       </c>
       <c r="M64" s="4" t="n">
         <v>8</v>
       </c>
       <c r="N64" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O64" s="2" t="n">
         <v>2</v>
@@ -3549,31 +3546,31 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D65" s="2" t="n">
-        <v>9.6</v>
+        <v>13.6</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F65" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G65" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="H65" s="2" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I65" s="2" t="n">
-        <v>48.8</v>
+        <v>3.3</v>
       </c>
       <c r="J65" s="2" t="n">
         <v>0</v>
@@ -3582,13 +3579,13 @@
         <v>0</v>
       </c>
       <c r="L65" s="3" t="n">
-        <v>0.99</v>
+        <v>2</v>
       </c>
       <c r="M65" s="4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N65" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O65" s="2" t="n">
         <v>2</v>
@@ -3596,46 +3593,46 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
-        <v>256</v>
+        <v>175</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D66" s="2" t="n">
-        <v>13.6</v>
+        <v>33.7</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>0.7</v>
+        <v>1.4</v>
       </c>
       <c r="F66" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="G66" s="2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H66" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I66" s="2" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="J66" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="3" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="M66" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N66" s="4" t="n">
         <v>5</v>
-      </c>
-      <c r="I66" s="2" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="J66" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K66" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="M66" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="N66" s="4" t="n">
-        <v>7</v>
       </c>
       <c r="O66" s="2" t="n">
         <v>2</v>
@@ -3643,87 +3640,87 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
-        <v>175</v>
+        <v>491</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>128</v>
+        <v>401</v>
       </c>
       <c r="D67" s="2" t="n">
-        <v>33.7</v>
+        <v>91.2</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>1.4</v>
+        <v>4.2</v>
       </c>
       <c r="F67" s="2" t="n">
-        <v>0.2</v>
+        <v>2.2</v>
       </c>
       <c r="G67" s="2" t="n">
-        <v>0.3</v>
+        <v>5.4</v>
       </c>
       <c r="H67" s="2" t="n">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="I67" s="2" t="n">
-        <v>15.7</v>
+        <v>0</v>
       </c>
       <c r="J67" s="2" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="K67" s="2" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="L67" s="3" t="n">
-        <v>1.65</v>
+        <v>2.67</v>
       </c>
       <c r="M67" s="4" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N67" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O67" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>401</v>
+        <v>540</v>
       </c>
       <c r="D68" s="2" t="n">
-        <v>91.2</v>
+        <v>59.6</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>4.2</v>
+        <v>7.2</v>
       </c>
       <c r="F68" s="2" t="n">
-        <v>2.2</v>
+        <v>30.3</v>
       </c>
       <c r="G68" s="2" t="n">
-        <v>5.4</v>
+        <v>1.6</v>
       </c>
       <c r="H68" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="I68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K68" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="I68" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J68" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K68" s="2" t="n">
-        <v>65</v>
-      </c>
       <c r="L68" s="3" t="n">
-        <v>2.67</v>
+        <v>5.99</v>
       </c>
       <c r="M68" s="4" t="n">
         <v>4</v>
@@ -3737,40 +3734,40 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>540</v>
+        <v>475</v>
       </c>
       <c r="D69" s="2" t="n">
-        <v>59.6</v>
+        <v>62.4</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>7.2</v>
+        <v>4.9</v>
       </c>
       <c r="F69" s="2" t="n">
-        <v>30.3</v>
+        <v>29.9</v>
       </c>
       <c r="G69" s="2" t="n">
-        <v>1.6</v>
+        <v>3.6</v>
       </c>
       <c r="H69" s="2" t="n">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="I69" s="2" t="n">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="J69" s="2" t="n">
-        <v>1.1</v>
+        <v>1.5</v>
       </c>
       <c r="K69" s="2" t="n">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="L69" s="3" t="n">
-        <v>5.99</v>
+        <v>11.29</v>
       </c>
       <c r="M69" s="4" t="n">
         <v>4</v>
@@ -3784,43 +3781,43 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="D70" s="2" t="n">
-        <v>62.4</v>
+        <v>81.4</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>4.9</v>
+        <v>1.1</v>
       </c>
       <c r="F70" s="2" t="n">
-        <v>29.9</v>
+        <v>13.6</v>
       </c>
       <c r="G70" s="2" t="n">
-        <v>3.6</v>
+        <v>1.2</v>
       </c>
       <c r="H70" s="2" t="n">
-        <v>107</v>
+        <v>17</v>
       </c>
       <c r="I70" s="2" t="n">
-        <v>2.1</v>
+        <v>0</v>
       </c>
       <c r="J70" s="2" t="n">
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
       <c r="K70" s="2" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="L70" s="3" t="n">
-        <v>11.29</v>
+        <v>8.39</v>
       </c>
       <c r="M70" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N70" s="4" t="n">
         <v>1</v>
@@ -3831,93 +3828,93 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
-        <v>499</v>
+        <v>561</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>449</v>
+        <v>76</v>
       </c>
       <c r="D71" s="2" t="n">
-        <v>81.4</v>
+        <v>13.6</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>1.1</v>
+        <v>4.8</v>
       </c>
       <c r="F71" s="2" t="n">
-        <v>13.6</v>
+        <v>0.5</v>
       </c>
       <c r="G71" s="2" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="H71" s="2" t="n">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="I71" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J71" s="2" t="n">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="K71" s="2" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="L71" s="3" t="n">
-        <v>8.39</v>
+        <v>0.699</v>
       </c>
       <c r="M71" s="4" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="N71" s="4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O71" s="2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>76</v>
+        <v>606</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>13.6</v>
+        <v>18.7</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>4.8</v>
+        <v>22.5</v>
       </c>
       <c r="F72" s="2" t="n">
-        <v>0.5</v>
+        <v>54</v>
       </c>
       <c r="G72" s="2" t="n">
         <v>1.3</v>
       </c>
       <c r="H72" s="2" t="n">
-        <v>42</v>
+        <v>159</v>
       </c>
       <c r="I72" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J72" s="2" t="n">
-        <v>0.7</v>
+        <v>2.1</v>
       </c>
       <c r="K72" s="2" t="n">
-        <v>2</v>
+        <v>376</v>
       </c>
       <c r="L72" s="3" t="n">
-        <v>0.699</v>
+        <v>3.89</v>
       </c>
       <c r="M72" s="4" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="N72" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O72" s="2" t="n">
         <v>6</v>
@@ -3925,90 +3922,90 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
-        <v>558</v>
+        <v>377</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>606</v>
+        <v>219</v>
       </c>
       <c r="D73" s="2" t="n">
-        <v>18.7</v>
+        <v>0</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>22.5</v>
+        <v>35.9</v>
       </c>
       <c r="F73" s="2" t="n">
-        <v>54</v>
+        <v>7.3</v>
       </c>
       <c r="G73" s="2" t="n">
-        <v>1.3</v>
+        <v>3</v>
       </c>
       <c r="H73" s="2" t="n">
-        <v>159</v>
+        <v>27</v>
       </c>
       <c r="I73" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J73" s="2" t="n">
-        <v>2.1</v>
+        <v>8.1</v>
       </c>
       <c r="K73" s="2" t="n">
-        <v>376</v>
+        <v>60</v>
       </c>
       <c r="L73" s="3" t="n">
-        <v>3.89</v>
+        <v>5.69</v>
       </c>
       <c r="M73" s="4" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="N73" s="4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O73" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
-        <v>377</v>
+        <v>488</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>219</v>
+        <v>146</v>
       </c>
       <c r="D74" s="2" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>35.9</v>
+        <v>13.3</v>
       </c>
       <c r="F74" s="2" t="n">
-        <v>7.3</v>
+        <v>9.5</v>
       </c>
       <c r="G74" s="2" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="H74" s="2" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="I74" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J74" s="2" t="n">
-        <v>8.1</v>
+        <v>1.2</v>
       </c>
       <c r="K74" s="2" t="n">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="L74" s="3" t="n">
-        <v>5.69</v>
+        <v>1.8</v>
       </c>
       <c r="M74" s="4" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N74" s="4" t="n">
         <v>7</v>
@@ -4019,43 +4016,43 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
-        <v>488</v>
+        <v>406</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>146</v>
+        <v>212</v>
       </c>
       <c r="D75" s="2" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>13.3</v>
+        <v>33.4</v>
       </c>
       <c r="F75" s="2" t="n">
-        <v>9.5</v>
+        <v>7.6</v>
       </c>
       <c r="G75" s="2" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="H75" s="2" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I75" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J75" s="2" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="K75" s="2" t="n">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="L75" s="3" t="n">
-        <v>1.8</v>
+        <v>2.49</v>
       </c>
       <c r="M75" s="4" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="N75" s="4" t="n">
         <v>7</v>
@@ -4066,43 +4063,43 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
-        <v>406</v>
+        <v>277</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>212</v>
+        <v>166</v>
       </c>
       <c r="D76" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>33.4</v>
+        <v>26.2</v>
       </c>
       <c r="F76" s="2" t="n">
-        <v>7.6</v>
+        <v>6</v>
       </c>
       <c r="G76" s="2" t="n">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="H76" s="2" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I76" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J76" s="2" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="K76" s="2" t="n">
-        <v>56</v>
+        <v>362</v>
       </c>
       <c r="L76" s="3" t="n">
-        <v>2.49</v>
+        <v>5.35</v>
       </c>
       <c r="M76" s="4" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="N76" s="4" t="n">
         <v>7</v>
@@ -4112,76 +4109,76 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="n">
-        <v>277</v>
-      </c>
-      <c r="B77" s="2" t="s">
+      <c r="A77" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="2" t="n">
-        <v>166</v>
-      </c>
-      <c r="D77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E77" s="2" t="n">
-        <v>26.2</v>
-      </c>
-      <c r="F77" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="G77" s="2" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="H77" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="I77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J77" s="2" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="K77" s="2" t="n">
-        <v>362</v>
-      </c>
-      <c r="L77" s="3" t="n">
-        <v>5.35</v>
-      </c>
-      <c r="M77" s="4" t="n">
-        <v>2</v>
+      <c r="C77" s="1" t="n">
+        <v>884</v>
+      </c>
+      <c r="D77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" s="1" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="M77" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="N77" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="O77" s="2" t="n">
-        <v>5</v>
+      <c r="O77" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>884</v>
+        <v>726</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F78" s="1" t="n">
-        <v>100</v>
+        <v>82.4</v>
       </c>
       <c r="G78" s="1" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H78" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I78" s="1" t="n">
         <v>0</v>
@@ -4190,10 +4187,10 @@
         <v>0</v>
       </c>
       <c r="K78" s="1" t="n">
-        <v>0</v>
+        <v>579</v>
       </c>
       <c r="L78" s="1" t="n">
-        <v>11.19</v>
+        <v>6.49</v>
       </c>
       <c r="M78" s="1" t="n">
         <v>1</v>
@@ -4202,53 +4199,6 @@
         <v>7</v>
       </c>
       <c r="O78" s="1" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
-        <v>261</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C79" s="1" t="n">
-        <v>726</v>
-      </c>
-      <c r="D79" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E79" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="F79" s="1" t="n">
-        <v>82.4</v>
-      </c>
-      <c r="G79" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H79" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I79" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K79" s="1" t="n">
-        <v>579</v>
-      </c>
-      <c r="L79" s="1" t="n">
-        <v>6.49</v>
-      </c>
-      <c r="M79" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N79" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O79" s="1" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>